<commit_message>
Quick Update 2026-02-24 19:59
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -2867,7 +2867,7 @@
         </is>
       </c>
       <c r="F55" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G55" s="3" t="inlineStr">
         <is>
@@ -2876,14 +2876,10 @@
       </c>
       <c r="H55" s="3" t="inlineStr">
         <is>
-          <t>Iterative</t>
-        </is>
-      </c>
-      <c r="I55" s="3" t="inlineStr">
-        <is>
           <t>Recursion</t>
         </is>
       </c>
+      <c r="I55" s="3" t="n"/>
       <c r="J55" s="3" t="n"/>
       <c r="K55" s="3" t="n"/>
     </row>
@@ -4415,7 +4411,7 @@
         </is>
       </c>
       <c r="F91" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G91" s="3" t="inlineStr">
         <is>
@@ -4424,14 +4420,10 @@
       </c>
       <c r="H91" s="3" t="inlineStr">
         <is>
-          <t>Iterative</t>
-        </is>
-      </c>
-      <c r="I91" s="3" t="inlineStr">
-        <is>
           <t>Recursion</t>
         </is>
       </c>
+      <c r="I91" s="3" t="n"/>
       <c r="J91" s="3" t="n"/>
       <c r="K91" s="3" t="n"/>
     </row>
@@ -4457,7 +4449,7 @@
         </is>
       </c>
       <c r="F92" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G92" s="3" t="inlineStr">
         <is>
@@ -4466,14 +4458,10 @@
       </c>
       <c r="H92" s="3" t="inlineStr">
         <is>
-          <t>Iterative</t>
-        </is>
-      </c>
-      <c r="I92" s="3" t="inlineStr">
-        <is>
           <t>Recursion</t>
         </is>
       </c>
+      <c r="I92" s="3" t="n"/>
       <c r="J92" s="3" t="n"/>
       <c r="K92" s="3" t="n"/>
     </row>

</xml_diff>

<commit_message>
Quick Update 2026-02-24 20:46
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="F14" s="6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3" t="inlineStr">
         <is>
@@ -1179,7 +1179,7 @@
         </is>
       </c>
       <c r="F15" s="6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Quick Update 2026-02-24 23:26
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="F42" s="6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G42" s="3" t="inlineStr">
         <is>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="I42" s="3" t="inlineStr">
         <is>
-          <t>Floyd's Algorithm</t>
+          <t>Hash Table</t>
         </is>
       </c>
       <c r="J42" s="3" t="n"/>
@@ -2359,7 +2359,7 @@
         </is>
       </c>
       <c r="F43" s="6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G43" s="3" t="inlineStr">
         <is>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="I43" s="3" t="inlineStr">
         <is>
-          <t>Floyd's Algorithm</t>
+          <t>Hash Table</t>
         </is>
       </c>
       <c r="J43" s="3" t="n"/>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 01:10
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -2990,7 +2990,7 @@
         </is>
       </c>
       <c r="F58" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G58" s="3" t="inlineStr">
         <is>
@@ -2999,12 +2999,12 @@
       </c>
       <c r="H58" s="3" t="inlineStr">
         <is>
-          <t>DFS</t>
+          <t>Depth-First Search</t>
         </is>
       </c>
       <c r="I58" s="3" t="inlineStr">
         <is>
-          <t>Recursion</t>
+          <t>Binary Tree</t>
         </is>
       </c>
       <c r="J58" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Quick Update 2026-02-25 01:12
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -3162,11 +3162,11 @@
         </is>
       </c>
       <c r="F62" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G62" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Hash Table</t>
         </is>
       </c>
       <c r="H62" s="3" t="inlineStr">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="I62" s="3" t="inlineStr">
         <is>
-          <t>Frequency Count</t>
+          <t>Sorting</t>
         </is>
       </c>
       <c r="J62" s="3" t="inlineStr">
@@ -4487,11 +4487,11 @@
         </is>
       </c>
       <c r="F93" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G93" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Hash Table</t>
         </is>
       </c>
       <c r="H93" s="3" t="inlineStr">
@@ -4501,7 +4501,7 @@
       </c>
       <c r="I93" s="3" t="inlineStr">
         <is>
-          <t>Frequency Count</t>
+          <t>Sorting</t>
         </is>
       </c>
       <c r="J93" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Quick Update 2026-02-25 02:03
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -3254,17 +3254,17 @@
       </c>
       <c r="G64" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H64" s="3" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>Binary Search</t>
         </is>
       </c>
       <c r="I64" s="3" t="inlineStr">
         <is>
-          <t>Frequency Count</t>
+          <t>Matrix</t>
         </is>
       </c>
       <c r="J64" s="3" t="n"/>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 03:01
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-18600" yWindow="-12375" windowWidth="38700" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Files" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Files'!$A$1:$K$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Files'!$A$1:$K$107</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -43,6 +43,12 @@
       <b val="1"/>
       <color rgb="FF9C0006"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <color rgb="FF1F2328"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="8">
@@ -110,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -136,6 +142,10 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,18 +511,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="10.5703125" customWidth="1" min="1" max="1"/>
-    <col width="20.5703125" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="20.5703125" customWidth="1" style="9" min="2" max="2"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
     <col width="52" customWidth="1" min="4" max="4"/>
     <col width="112.28515625" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
@@ -576,10 +586,10 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.95" customHeight="1">
+    <row r="2" hidden="1" ht="15.95" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -615,15 +625,11 @@
           <t>Hash Table</t>
         </is>
       </c>
-      <c r="I2" s="3" t="inlineStr">
-        <is>
-          <t>One Pass</t>
-        </is>
-      </c>
+      <c r="I2" s="3" t="n"/>
       <c r="J2" s="3" t="n"/>
       <c r="K2" s="3" t="n"/>
     </row>
-    <row r="3" ht="15.95" customHeight="1">
+    <row r="3" hidden="1" ht="15.95" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
           <t>X</t>
@@ -670,7 +676,7 @@
       <c r="J3" s="3" t="n"/>
       <c r="K3" s="3" t="n"/>
     </row>
-    <row r="4" ht="15.95" customHeight="1">
+    <row r="4" hidden="1" ht="15.95" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
           <t>X</t>
@@ -1031,7 +1037,12 @@
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
-    <row r="12" hidden="1" ht="15.95" customHeight="1">
+    <row r="12" ht="15.95" customHeight="1">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
           <t>LC0020</t>
@@ -1053,16 +1064,16 @@
         </is>
       </c>
       <c r="F12" s="6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G12" s="3" t="inlineStr">
         <is>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
           <t>Stack</t>
-        </is>
-      </c>
-      <c r="H12" s="3" t="inlineStr">
-        <is>
-          <t>String</t>
         </is>
       </c>
       <c r="I12" s="3" t="inlineStr">
@@ -1073,7 +1084,12 @@
       <c r="J12" s="3" t="n"/>
       <c r="K12" s="3" t="n"/>
     </row>
-    <row r="13" hidden="1" ht="15.95" customHeight="1">
+    <row r="13" ht="15.95" customHeight="1">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
           <t>LC0020</t>
@@ -1095,16 +1111,16 @@
         </is>
       </c>
       <c r="F13" s="6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
           <t>Stack</t>
-        </is>
-      </c>
-      <c r="H13" s="3" t="inlineStr">
-        <is>
-          <t>String</t>
         </is>
       </c>
       <c r="I13" s="3" t="inlineStr">
@@ -1116,6 +1132,11 @@
       <c r="K13" s="3" t="n"/>
     </row>
     <row r="14" hidden="1" ht="15.95" customHeight="1">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
           <t>LC0021</t>
@@ -1158,6 +1179,11 @@
       <c r="K14" s="3" t="n"/>
     </row>
     <row r="15" hidden="1" ht="15.95" customHeight="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
           <t>LC0021</t>
@@ -1585,7 +1611,12 @@
       <c r="J24" s="3" t="n"/>
       <c r="K24" s="3" t="n"/>
     </row>
-    <row r="25" ht="15.95" customHeight="1">
+    <row r="25" hidden="1" ht="15.95" customHeight="1">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
           <t>LC0070</t>
@@ -1627,7 +1658,12 @@
       <c r="J25" s="3" t="n"/>
       <c r="K25" s="3" t="n"/>
     </row>
-    <row r="26" ht="15.95" customHeight="1">
+    <row r="26" hidden="1" ht="15.95" customHeight="1">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
           <t>LC0070</t>
@@ -1669,7 +1705,12 @@
       <c r="J26" s="3" t="n"/>
       <c r="K26" s="3" t="n"/>
     </row>
-    <row r="27" ht="15.95" customHeight="1">
+    <row r="27" hidden="1" ht="15.95" customHeight="1">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
           <t>LC0070</t>
@@ -1711,7 +1752,12 @@
       <c r="J27" s="3" t="n"/>
       <c r="K27" s="3" t="n"/>
     </row>
-    <row r="28" ht="15.95" customHeight="1">
+    <row r="28" hidden="1" ht="15.95" customHeight="1">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
           <t>LC0070</t>
@@ -1967,71 +2013,67 @@
       </c>
       <c r="K33" s="3" t="n"/>
     </row>
-    <row r="34" ht="15.95" customHeight="1">
+    <row r="34" hidden="1" ht="15.95" customHeight="1">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>LC0100</t>
-        </is>
-      </c>
-      <c r="C34" s="2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="D34" s="3" t="inlineStr">
-        <is>
-          <t>000037.LC0100.same-tree.py</t>
-        </is>
-      </c>
-      <c r="E34" s="3" t="inlineStr">
-        <is>
-          <t>C:\DataMajor\practice\000037.LC0100.same-tree.py</t>
-        </is>
-      </c>
-      <c r="F34" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G34" s="3" t="inlineStr">
-        <is>
-          <t>Tree</t>
-        </is>
-      </c>
-      <c r="H34" s="3" t="inlineStr">
-        <is>
-          <t>Depth-First Search</t>
-        </is>
-      </c>
-      <c r="I34" s="3" t="inlineStr">
-        <is>
-          <t>Binary Tree</t>
-        </is>
-      </c>
+          <t>LC0083</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="D34" s="3" t="n"/>
+      <c r="E34" s="10" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\001Study\playground\group1\83.ipynb</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="10" t="inlineStr">
+        <is>
+          <t>Linked List"</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="n"/>
+      <c r="I34" s="3" t="n"/>
       <c r="J34" s="3" t="n"/>
       <c r="K34" s="3" t="n"/>
     </row>
     <row r="35" hidden="1" ht="15.95" customHeight="1">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>LC0102</t>
+          <t>LC0100</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>000010.LC0102.level-order-traversal.alt-deque.py</t>
+          <t>000037.LC0100.same-tree.py</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000010.LC0102.level-order-traversal.alt-deque.py</t>
-        </is>
-      </c>
-      <c r="F35" s="6" t="n">
-        <v>4</v>
+          <t>C:\DataMajor\practice\000037.LC0100.same-tree.py</t>
+        </is>
+      </c>
+      <c r="F35" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="G35" s="3" t="inlineStr">
         <is>
@@ -2040,12 +2082,12 @@
       </c>
       <c r="H35" s="3" t="inlineStr">
         <is>
-          <t>BFS</t>
+          <t>Depth-First Search</t>
         </is>
       </c>
       <c r="I35" s="3" t="inlineStr">
         <is>
-          <t>Queue</t>
+          <t>Binary Tree</t>
         </is>
       </c>
       <c r="J35" s="3" t="n"/>
@@ -2064,12 +2106,12 @@
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>000010.LC0102.level-order-traversal.py</t>
+          <t>000010.LC0102.level-order-traversal.alt-deque.py</t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000010.LC0102.level-order-traversal.py</t>
+          <t>C:\DataMajor\practice\000010.LC0102.level-order-traversal.alt-deque.py</t>
         </is>
       </c>
       <c r="F36" s="6" t="n">
@@ -2093,91 +2135,101 @@
       <c r="J36" s="3" t="n"/>
       <c r="K36" s="3" t="n"/>
     </row>
-    <row r="37" ht="15.95" customHeight="1">
+    <row r="37" hidden="1" ht="15.95" customHeight="1">
       <c r="B37" s="2" t="inlineStr">
         <is>
+          <t>LC0102</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="inlineStr">
+        <is>
+          <t>000010.LC0102.level-order-traversal.py</t>
+        </is>
+      </c>
+      <c r="E37" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\000010.LC0102.level-order-traversal.py</t>
+        </is>
+      </c>
+      <c r="F37" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G37" s="3" t="inlineStr">
+        <is>
+          <t>Tree</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>BFS</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>Queue</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="n"/>
+      <c r="K37" s="3" t="n"/>
+    </row>
+    <row r="38" hidden="1" ht="15.95" customHeight="1">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
           <t>LC0104</t>
         </is>
       </c>
-      <c r="C37" s="2" t="inlineStr">
+      <c r="C38" s="2" t="inlineStr">
         <is>
           <t>104</t>
         </is>
       </c>
-      <c r="D37" s="3" t="inlineStr">
+      <c r="D38" s="3" t="inlineStr">
         <is>
           <t>000009.LC0104.max-depth-binary-tree.py</t>
         </is>
       </c>
-      <c r="E37" s="3" t="inlineStr">
+      <c r="E38" s="3" t="inlineStr">
         <is>
           <t>C:\DataMajor\practice\000009.LC0104.max-depth-binary-tree.py</t>
         </is>
       </c>
-      <c r="F37" s="4" t="n">
+      <c r="F38" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G37" s="3" t="inlineStr">
+      <c r="G38" s="3" t="inlineStr">
         <is>
           <t>Tree</t>
         </is>
       </c>
-      <c r="H37" s="3" t="inlineStr">
+      <c r="H38" s="3" t="inlineStr">
         <is>
           <t>Depth-First Search</t>
         </is>
       </c>
-      <c r="I37" s="3" t="inlineStr">
+      <c r="I38" s="3" t="inlineStr">
         <is>
           <t>Breadth-First Search</t>
         </is>
       </c>
-      <c r="J37" s="3" t="inlineStr">
-        <is>
-          <t>BFS</t>
-        </is>
-      </c>
-      <c r="K37" s="3" t="n"/>
-    </row>
-    <row r="38" ht="15.95" customHeight="1">
-      <c r="B38" s="2" t="inlineStr">
-        <is>
-          <t>LC0121</t>
-        </is>
-      </c>
-      <c r="C38" s="2" t="inlineStr">
-        <is>
-          <t>121</t>
-        </is>
-      </c>
-      <c r="D38" s="3" t="inlineStr">
-        <is>
-          <t>000029.LC0121.best-time-buy-sell.redo.py</t>
-        </is>
-      </c>
-      <c r="E38" s="3" t="inlineStr">
-        <is>
-          <t>C:\DataMajor\practice\000029.LC0121.best-time-buy-sell.redo.py</t>
-        </is>
-      </c>
-      <c r="F38" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
-        </is>
-      </c>
-      <c r="H38" s="3" t="inlineStr">
-        <is>
-          <t>Dynamic Programming</t>
-        </is>
-      </c>
-      <c r="I38" s="3" t="n"/>
       <c r="J38" s="3" t="n"/>
       <c r="K38" s="3" t="n"/>
     </row>
-    <row r="39" ht="15.95" customHeight="1">
+    <row r="39" hidden="1" ht="15.95" customHeight="1">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
           <t>LC0121</t>
@@ -2190,12 +2242,12 @@
       </c>
       <c r="D39" s="3" t="inlineStr">
         <is>
-          <t>000003.LC0121.best-time-buy-sell.py</t>
+          <t>000029.LC0121.best-time-buy-sell.redo.py</t>
         </is>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000003.LC0121.best-time-buy-sell.py</t>
+          <t>C:\DataMajor\practice\000029.LC0121.best-time-buy-sell.redo.py</t>
         </is>
       </c>
       <c r="F39" s="4" t="n">
@@ -2215,7 +2267,12 @@
       <c r="J39" s="3" t="n"/>
       <c r="K39" s="3" t="n"/>
     </row>
-    <row r="40" ht="15.95" customHeight="1">
+    <row r="40" hidden="1" ht="15.95" customHeight="1">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
           <t>LC0121</t>
@@ -2228,12 +2285,12 @@
       </c>
       <c r="D40" s="3" t="inlineStr">
         <is>
-          <t>000023.LC0121.best-time-buy-sell.redo.py</t>
+          <t>000003.LC0121.best-time-buy-sell.py</t>
         </is>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000023.LC0121.best-time-buy-sell.redo.py</t>
+          <t>C:\DataMajor\practice\000003.LC0121.best-time-buy-sell.py</t>
         </is>
       </c>
       <c r="F40" s="4" t="n">
@@ -2254,90 +2311,96 @@
       <c r="K40" s="3" t="n"/>
     </row>
     <row r="41" hidden="1" ht="15.95" customHeight="1">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>LC0128</t>
+          <t>LC0121</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>121</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
         <is>
-          <t>00036_LeetCode128_LongestConsecutiveSequence.ipynb</t>
+          <t>000023.LC0121.best-time-buy-sell.redo.py</t>
         </is>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00036_LeetCode128_LongestConsecutiveSequence.ipynb</t>
-        </is>
-      </c>
-      <c r="F41" s="5" t="n">
-        <v>5</v>
+          <t>C:\DataMajor\practice\000023.LC0121.best-time-buy-sell.redo.py</t>
+        </is>
+      </c>
+      <c r="F41" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="G41" s="3" t="inlineStr">
         <is>
-          <t>Hash Set</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H41" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
-        </is>
-      </c>
-      <c r="I41" s="3" t="inlineStr">
-        <is>
-          <t>Union Find</t>
-        </is>
-      </c>
+          <t>Dynamic Programming</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="n"/>
       <c r="J41" s="3" t="n"/>
       <c r="K41" s="3" t="n"/>
     </row>
     <row r="42" hidden="1" ht="15.95" customHeight="1">
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>LC0141</t>
+          <t>LC0128</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>128</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
         <is>
-          <t>000030.LC0141.linked-list-cycle.py</t>
+          <t>00036_LeetCode128_LongestConsecutiveSequence.ipynb</t>
         </is>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000030.LC0141.linked-list-cycle.py</t>
-        </is>
-      </c>
-      <c r="F42" s="6" t="n">
-        <v>1</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00036_LeetCode128_LongestConsecutiveSequence.ipynb</t>
+        </is>
+      </c>
+      <c r="F42" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G42" s="3" t="inlineStr">
         <is>
-          <t>Linked List</t>
+          <t>Hash Set</t>
         </is>
       </c>
       <c r="H42" s="3" t="inlineStr">
         <is>
-          <t>Two Pointers</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="I42" s="3" t="inlineStr">
         <is>
-          <t>Hash Table</t>
+          <t>Union Find</t>
         </is>
       </c>
       <c r="J42" s="3" t="n"/>
       <c r="K42" s="3" t="n"/>
     </row>
     <row r="43" hidden="1" ht="15.95" customHeight="1">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
           <t>LC0141</t>
@@ -2350,12 +2413,12 @@
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>000030.LC0141.linked-list-cycle.study.py</t>
+          <t>000030.LC0141.linked-list-cycle.py</t>
         </is>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000030.LC0141.linked-list-cycle.study.py</t>
+          <t>C:\DataMajor\practice\000030.LC0141.linked-list-cycle.py</t>
         </is>
       </c>
       <c r="F43" s="6" t="n">
@@ -2363,144 +2426,103 @@
       </c>
       <c r="G43" s="3" t="inlineStr">
         <is>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
           <t>Linked List</t>
         </is>
       </c>
-      <c r="H43" s="3" t="inlineStr">
+      <c r="I43" s="3" t="inlineStr">
         <is>
           <t>Two Pointers</t>
-        </is>
-      </c>
-      <c r="I43" s="3" t="inlineStr">
-        <is>
-          <t>Hash Table</t>
         </is>
       </c>
       <c r="J43" s="3" t="n"/>
       <c r="K43" s="3" t="n"/>
     </row>
     <row r="44" hidden="1" ht="15.95" customHeight="1">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>LC0146</t>
+          <t>LC0141</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>141</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>00037_LeetCode146_LRUCache.ipynb</t>
+          <t>000030.LC0141.linked-list-cycle.study.py</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00037_LeetCode146_LRUCache.ipynb</t>
-        </is>
-      </c>
-      <c r="F44" s="8" t="n">
-        <v>7</v>
+          <t>C:\DataMajor\practice\000030.LC0141.linked-list-cycle.study.py</t>
+        </is>
+      </c>
+      <c r="F44" s="6" t="n">
+        <v>1</v>
       </c>
       <c r="G44" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Linked List</t>
         </is>
       </c>
       <c r="H44" s="3" t="inlineStr">
         <is>
-          <t>Doubly Linked List</t>
+          <t>Two Pointers</t>
         </is>
       </c>
       <c r="I44" s="3" t="inlineStr">
         <is>
-          <t>Design</t>
-        </is>
-      </c>
-      <c r="J44" s="3" t="inlineStr">
-        <is>
-          <t>OrderedDict</t>
-        </is>
-      </c>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="n"/>
       <c r="K44" s="3" t="n"/>
     </row>
     <row r="45" hidden="1" ht="15.95" customHeight="1">
-      <c r="B45" s="2" t="inlineStr">
-        <is>
-          <t>LC0150</t>
-        </is>
-      </c>
-      <c r="C45" s="2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="inlineStr">
-        <is>
-          <t>00038_LeetCode150_EvaluateReversePolishNotation.ipynb</t>
-        </is>
-      </c>
-      <c r="E45" s="3" t="inlineStr">
-        <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00038_LeetCode150_EvaluateReversePolishNotation.ipynb</t>
-        </is>
-      </c>
-      <c r="F45" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G45" s="3" t="inlineStr">
-        <is>
-          <t>Stack</t>
-        </is>
-      </c>
-      <c r="H45" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
-        </is>
-      </c>
-      <c r="I45" s="3" t="inlineStr">
-        <is>
-          <t>Math</t>
-        </is>
-      </c>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="n"/>
+      <c r="C45" s="2" t="n">
+        <v>142</v>
+      </c>
+      <c r="D45" s="3" t="n"/>
+      <c r="E45" s="3" t="n"/>
+      <c r="F45" s="6" t="n"/>
+      <c r="G45" s="3" t="n"/>
+      <c r="H45" s="3" t="n"/>
+      <c r="I45" s="3" t="n"/>
       <c r="J45" s="3" t="n"/>
       <c r="K45" s="3" t="n"/>
     </row>
     <row r="46" hidden="1" ht="15.95" customHeight="1">
-      <c r="B46" s="2" t="inlineStr">
-        <is>
-          <t>LC0153</t>
-        </is>
-      </c>
-      <c r="C46" s="2" t="inlineStr">
-        <is>
-          <t>153</t>
-        </is>
-      </c>
-      <c r="D46" s="3" t="inlineStr">
-        <is>
-          <t>00153_LeetCode153_FindMinimumInRotatedSortedArray.ipynb</t>
-        </is>
-      </c>
-      <c r="E46" s="3" t="inlineStr">
-        <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00153_LeetCode153_FindMinimumInRotatedSortedArray.ipynb</t>
-        </is>
-      </c>
-      <c r="F46" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G46" s="3" t="inlineStr">
-        <is>
-          <t>Binary Search</t>
-        </is>
-      </c>
-      <c r="H46" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
-        </is>
-      </c>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="n"/>
+      <c r="C46" s="2" t="n">
+        <v>143</v>
+      </c>
+      <c r="D46" s="3" t="n"/>
+      <c r="E46" s="3" t="n"/>
+      <c r="F46" s="6" t="n"/>
+      <c r="G46" s="3" t="n"/>
+      <c r="H46" s="3" t="n"/>
       <c r="I46" s="3" t="n"/>
       <c r="J46" s="3" t="n"/>
       <c r="K46" s="3" t="n"/>
@@ -2508,68 +2530,76 @@
     <row r="47" hidden="1" ht="15.95" customHeight="1">
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>LC0153</t>
+          <t>LC0146</t>
         </is>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>146</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
         <is>
-          <t>leetCode153.py</t>
+          <t>00037_LeetCode146_LRUCache.ipynb</t>
         </is>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Temp\leetCode153.py</t>
-        </is>
-      </c>
-      <c r="F47" s="5" t="n">
-        <v>5</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00037_LeetCode146_LRUCache.ipynb</t>
+        </is>
+      </c>
+      <c r="F47" s="8" t="n">
+        <v>7</v>
       </c>
       <c r="G47" s="3" t="inlineStr">
         <is>
-          <t>Binary Search</t>
+          <t>Hash Map</t>
         </is>
       </c>
       <c r="H47" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
-        </is>
-      </c>
-      <c r="I47" s="3" t="n"/>
-      <c r="J47" s="3" t="n"/>
+          <t>Doubly Linked List</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>Design</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>OrderedDict</t>
+        </is>
+      </c>
       <c r="K47" s="3" t="n"/>
     </row>
     <row r="48" hidden="1" ht="15.95" customHeight="1">
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>LC0154</t>
+          <t>LC0150</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>150</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>00154_LeetCode154_FindMinimumInRotatedSortedArrayII.ipynb</t>
+          <t>00038_LeetCode150_EvaluateReversePolishNotation.ipynb</t>
         </is>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00154_LeetCode154_FindMinimumInRotatedSortedArrayII.ipynb</t>
-        </is>
-      </c>
-      <c r="F48" s="8" t="n">
-        <v>7</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00038_LeetCode150_EvaluateReversePolishNotation.ipynb</t>
+        </is>
+      </c>
+      <c r="F48" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G48" s="3" t="inlineStr">
         <is>
-          <t>Binary Search</t>
+          <t>Stack</t>
         </is>
       </c>
       <c r="H48" s="3" t="inlineStr">
@@ -2579,7 +2609,7 @@
       </c>
       <c r="I48" s="3" t="inlineStr">
         <is>
-          <t>Duplicates</t>
+          <t>Math</t>
         </is>
       </c>
       <c r="J48" s="3" t="n"/>
@@ -2588,72 +2618,68 @@
     <row r="49" hidden="1" ht="15.95" customHeight="1">
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>LC0155</t>
+          <t>LC0153</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>153</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>00039_LeetCode155_MinStack.ipynb</t>
+          <t>00153_LeetCode153_FindMinimumInRotatedSortedArray.ipynb</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00039_LeetCode155_MinStack.ipynb</t>
-        </is>
-      </c>
-      <c r="F49" s="6" t="n">
-        <v>4</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00153_LeetCode153_FindMinimumInRotatedSortedArray.ipynb</t>
+        </is>
+      </c>
+      <c r="F49" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G49" s="3" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>Binary Search</t>
         </is>
       </c>
       <c r="H49" s="3" t="inlineStr">
         <is>
-          <t>Design</t>
-        </is>
-      </c>
-      <c r="I49" s="3" t="inlineStr">
-        <is>
-          <t>Auxiliary Stack</t>
-        </is>
-      </c>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="n"/>
       <c r="J49" s="3" t="n"/>
       <c r="K49" s="3" t="n"/>
     </row>
     <row r="50" hidden="1" ht="15.95" customHeight="1">
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>LC0167</t>
+          <t>LC0153</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>153</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
         <is>
-          <t>000011.LC0167.two-sum-ii.py</t>
+          <t>leetCode153.py</t>
         </is>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000011.LC0167.two-sum-ii.py</t>
-        </is>
-      </c>
-      <c r="F50" s="6" t="n">
-        <v>3</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Temp\leetCode153.py</t>
+        </is>
+      </c>
+      <c r="F50" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G50" s="3" t="inlineStr">
         <is>
-          <t>Two Pointers</t>
+          <t>Binary Search</t>
         </is>
       </c>
       <c r="H50" s="3" t="inlineStr">
@@ -2661,41 +2687,37 @@
           <t>Array</t>
         </is>
       </c>
-      <c r="I50" s="3" t="inlineStr">
-        <is>
-          <t>Binary Search</t>
-        </is>
-      </c>
+      <c r="I50" s="3" t="n"/>
       <c r="J50" s="3" t="n"/>
       <c r="K50" s="3" t="n"/>
     </row>
     <row r="51" hidden="1" ht="15.95" customHeight="1">
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>LC0198</t>
+          <t>LC0154</t>
         </is>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>198</t>
+          <t>154</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>000016.LC0198.house-robber.py</t>
+          <t>00154_LeetCode154_FindMinimumInRotatedSortedArrayII.ipynb</t>
         </is>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000016.LC0198.house-robber.py</t>
-        </is>
-      </c>
-      <c r="F51" s="6" t="n">
-        <v>4</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00154_LeetCode154_FindMinimumInRotatedSortedArrayII.ipynb</t>
+        </is>
+      </c>
+      <c r="F51" s="8" t="n">
+        <v>7</v>
       </c>
       <c r="G51" s="3" t="inlineStr">
         <is>
-          <t>Dynamic Programming</t>
+          <t>Binary Search</t>
         </is>
       </c>
       <c r="H51" s="3" t="inlineStr">
@@ -2703,205 +2725,201 @@
           <t>Array</t>
         </is>
       </c>
-      <c r="I51" s="3" t="n"/>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>Duplicates</t>
+        </is>
+      </c>
       <c r="J51" s="3" t="n"/>
       <c r="K51" s="3" t="n"/>
     </row>
     <row r="52" hidden="1" ht="15.95" customHeight="1">
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>LC0200</t>
+          <t>LC0155</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>155</t>
         </is>
       </c>
       <c r="D52" s="3" t="inlineStr">
         <is>
-          <t>05_LeetCode_200.ipynb</t>
+          <t>00039_LeetCode155_MinStack.ipynb</t>
         </is>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\playground\DSA\05_LeetCode_200.ipynb</t>
-        </is>
-      </c>
-      <c r="F52" s="5" t="n">
-        <v>5</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00039_LeetCode155_MinStack.ipynb</t>
+        </is>
+      </c>
+      <c r="F52" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="G52" s="3" t="inlineStr">
         <is>
-          <t>DFS</t>
+          <t>Stack</t>
         </is>
       </c>
       <c r="H52" s="3" t="inlineStr">
         <is>
-          <t>BFS</t>
+          <t>Design</t>
         </is>
       </c>
       <c r="I52" s="3" t="inlineStr">
         <is>
-          <t>Matrix</t>
-        </is>
-      </c>
-      <c r="J52" s="3" t="inlineStr">
-        <is>
-          <t>Union Find</t>
-        </is>
-      </c>
+          <t>Auxiliary Stack</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="n"/>
       <c r="K52" s="3" t="n"/>
     </row>
-    <row r="53" hidden="1" ht="15.95" customHeight="1">
+    <row r="53" ht="15.95" customHeight="1">
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>LC0200</t>
+          <t>LC0167</t>
         </is>
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>167</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>000015.LC0200.number-of-islands.py</t>
+          <t>000011.LC0167.two-sum-ii.py</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000015.LC0200.number-of-islands.py</t>
-        </is>
-      </c>
-      <c r="F53" s="5" t="n">
-        <v>5</v>
+          <t>C:\DataMajor\practice\000011.LC0167.two-sum-ii.py</t>
+        </is>
+      </c>
+      <c r="F53" s="6" t="n">
+        <v>3</v>
       </c>
       <c r="G53" s="3" t="inlineStr">
         <is>
-          <t>DFS</t>
+          <t>Two Pointers</t>
         </is>
       </c>
       <c r="H53" s="3" t="inlineStr">
         <is>
-          <t>BFS</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="I53" s="3" t="inlineStr">
         <is>
-          <t>Matrix</t>
-        </is>
-      </c>
-      <c r="J53" s="3" t="inlineStr">
-        <is>
-          <t>Union Find</t>
-        </is>
-      </c>
+          <t>Binary Search</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="n"/>
       <c r="K53" s="3" t="n"/>
     </row>
     <row r="54" hidden="1" ht="15.95" customHeight="1">
       <c r="B54" s="2" t="inlineStr">
         <is>
+          <t>LC0198</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>198</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="inlineStr">
+        <is>
+          <t>000016.LC0198.house-robber.py</t>
+        </is>
+      </c>
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\000016.LC0198.house-robber.py</t>
+        </is>
+      </c>
+      <c r="F54" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G54" s="3" t="inlineStr">
+        <is>
+          <t>Dynamic Programming</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="n"/>
+      <c r="J54" s="3" t="n"/>
+      <c r="K54" s="3" t="n"/>
+    </row>
+    <row r="55" hidden="1" ht="15.95" customHeight="1">
+      <c r="B55" s="2" t="inlineStr">
+        <is>
           <t>LC0200</t>
         </is>
       </c>
-      <c r="C54" s="2" t="inlineStr">
+      <c r="C55" s="2" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
-      <c r="D54" s="3" t="inlineStr">
-        <is>
-          <t>00040_LeetCode200_NumberOfIslands.ipynb</t>
-        </is>
-      </c>
-      <c r="E54" s="3" t="inlineStr">
-        <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00040_LeetCode200_NumberOfIslands.ipynb</t>
-        </is>
-      </c>
-      <c r="F54" s="5" t="n">
+      <c r="D55" s="3" t="inlineStr">
+        <is>
+          <t>05_LeetCode_200.ipynb</t>
+        </is>
+      </c>
+      <c r="E55" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\playground\DSA\05_LeetCode_200.ipynb</t>
+        </is>
+      </c>
+      <c r="F55" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G54" s="3" t="inlineStr">
+      <c r="G55" s="3" t="inlineStr">
         <is>
           <t>DFS</t>
         </is>
       </c>
-      <c r="H54" s="3" t="inlineStr">
+      <c r="H55" s="3" t="inlineStr">
         <is>
           <t>BFS</t>
         </is>
       </c>
-      <c r="I54" s="3" t="inlineStr">
+      <c r="I55" s="3" t="inlineStr">
         <is>
           <t>Matrix</t>
         </is>
       </c>
-      <c r="J54" s="3" t="inlineStr">
+      <c r="J55" s="3" t="inlineStr">
         <is>
           <t>Union Find</t>
         </is>
       </c>
-      <c r="K54" s="3" t="n"/>
-    </row>
-    <row r="55" ht="15.95" customHeight="1">
-      <c r="B55" s="2" t="inlineStr">
-        <is>
-          <t>LC0206</t>
-        </is>
-      </c>
-      <c r="C55" s="2" t="inlineStr">
-        <is>
-          <t>206</t>
-        </is>
-      </c>
-      <c r="D55" s="3" t="inlineStr">
-        <is>
-          <t>00041_LeetCode206_ReverseLinkedList.ipynb</t>
-        </is>
-      </c>
-      <c r="E55" s="3" t="inlineStr">
-        <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00041_LeetCode206_ReverseLinkedList.ipynb</t>
-        </is>
-      </c>
-      <c r="F55" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G55" s="3" t="inlineStr">
-        <is>
-          <t>Linked List</t>
-        </is>
-      </c>
-      <c r="H55" s="3" t="inlineStr">
-        <is>
-          <t>Recursion</t>
-        </is>
-      </c>
-      <c r="I55" s="3" t="n"/>
-      <c r="J55" s="3" t="n"/>
       <c r="K55" s="3" t="n"/>
     </row>
     <row r="56" hidden="1" ht="15.95" customHeight="1">
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>LC0209</t>
+          <t>LC0200</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>200</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
         <is>
-          <t>00018_LeetCode209_MinimumSizeSubarraySum.ipynb</t>
+          <t>000015.LC0200.number-of-islands.py</t>
         </is>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00018_LeetCode209_MinimumSizeSubarraySum.ipynb</t>
+          <t>C:\DataMajor\practice\000015.LC0200.number-of-islands.py</t>
         </is>
       </c>
       <c r="F56" s="5" t="n">
@@ -2909,218 +2927,214 @@
       </c>
       <c r="G56" s="3" t="inlineStr">
         <is>
-          <t>Sliding Window</t>
+          <t>DFS</t>
         </is>
       </c>
       <c r="H56" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
+          <t>BFS</t>
         </is>
       </c>
       <c r="I56" s="3" t="inlineStr">
         <is>
-          <t>Two Pointers</t>
-        </is>
-      </c>
-      <c r="J56" s="3" t="n"/>
+          <t>Matrix</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr">
+        <is>
+          <t>Union Find</t>
+        </is>
+      </c>
       <c r="K56" s="3" t="n"/>
     </row>
     <row r="57" hidden="1" ht="15.95" customHeight="1">
-      <c r="A57" t="inlineStr">
+      <c r="B57" s="2" t="inlineStr">
+        <is>
+          <t>LC0200</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D57" s="3" t="inlineStr">
+        <is>
+          <t>00040_LeetCode200_NumberOfIslands.ipynb</t>
+        </is>
+      </c>
+      <c r="E57" s="3" t="inlineStr">
+        <is>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00040_LeetCode200_NumberOfIslands.ipynb</t>
+        </is>
+      </c>
+      <c r="F57" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G57" s="3" t="inlineStr">
+        <is>
+          <t>DFS</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>BFS</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>Matrix</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr">
+        <is>
+          <t>Union Find</t>
+        </is>
+      </c>
+      <c r="K57" s="3" t="n"/>
+    </row>
+    <row r="58" hidden="1" ht="15.95" customHeight="1">
+      <c r="A58" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="B57" s="2" t="inlineStr">
-        <is>
-          <t>LC0217</t>
-        </is>
-      </c>
-      <c r="C57" s="2" t="inlineStr">
-        <is>
-          <t>217</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="inlineStr">
-        <is>
-          <t>00014_LeetCode217_ContainsDuplicate.ipynb</t>
-        </is>
-      </c>
-      <c r="E57" s="3" t="inlineStr">
-        <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00014_LeetCode217_ContainsDuplicate.ipynb</t>
-        </is>
-      </c>
-      <c r="F57" s="4" t="n">
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>LC0203</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>203</v>
+      </c>
+      <c r="D58" s="3" t="n"/>
+      <c r="E58" s="10" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\001Study\playground\group1\203.ipynb</t>
+        </is>
+      </c>
+      <c r="F58" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G57" s="3" t="inlineStr">
-        <is>
-          <t>Hash Set</t>
-        </is>
-      </c>
-      <c r="H57" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
-        </is>
-      </c>
-      <c r="I57" s="3" t="n"/>
-      <c r="J57" s="3" t="n"/>
-      <c r="K57" s="3" t="n"/>
-    </row>
-    <row r="58" ht="15.95" customHeight="1">
-      <c r="B58" s="2" t="inlineStr">
-        <is>
-          <t>LC0226</t>
-        </is>
-      </c>
-      <c r="C58" s="2" t="inlineStr">
-        <is>
-          <t>226</t>
-        </is>
-      </c>
-      <c r="D58" s="3" t="inlineStr">
-        <is>
-          <t>000022.LC0226.invert-binary-tree.py</t>
-        </is>
-      </c>
-      <c r="E58" s="3" t="inlineStr">
-        <is>
-          <t>C:\DataMajor\practice\000022.LC0226.invert-binary-tree.py</t>
-        </is>
-      </c>
-      <c r="F58" s="4" t="n">
+      <c r="G58" s="3" t="n"/>
+      <c r="H58" s="3" t="n"/>
+      <c r="I58" s="3" t="n"/>
+      <c r="J58" s="3" t="n"/>
+      <c r="K58" s="3" t="n"/>
+    </row>
+    <row r="59" hidden="1" ht="15.95" customHeight="1">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
+        <is>
+          <t>LC0206</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="inlineStr">
+        <is>
+          <t>206</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>00041_LeetCode206_ReverseLinkedList.ipynb</t>
+        </is>
+      </c>
+      <c r="E59" s="3" t="inlineStr">
+        <is>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00041_LeetCode206_ReverseLinkedList.ipynb</t>
+        </is>
+      </c>
+      <c r="F59" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G58" s="3" t="inlineStr">
-        <is>
-          <t>Tree</t>
-        </is>
-      </c>
-      <c r="H58" s="3" t="inlineStr">
-        <is>
-          <t>Depth-First Search</t>
-        </is>
-      </c>
-      <c r="I58" s="3" t="inlineStr">
-        <is>
-          <t>Binary Tree</t>
-        </is>
-      </c>
-      <c r="J58" s="3" t="inlineStr">
-        <is>
-          <t>BFS</t>
-        </is>
-      </c>
-      <c r="K58" s="3" t="n"/>
-    </row>
-    <row r="59" hidden="1" ht="15.95" customHeight="1">
-      <c r="B59" s="2" t="inlineStr">
-        <is>
-          <t>LC0227</t>
-        </is>
-      </c>
-      <c r="C59" s="2" t="inlineStr">
-        <is>
-          <t>227</t>
-        </is>
-      </c>
-      <c r="D59" s="3" t="inlineStr">
-        <is>
-          <t>00042_LeetCode227_BasicCalculatorII.ipynb</t>
-        </is>
-      </c>
-      <c r="E59" s="3" t="inlineStr">
-        <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00042_LeetCode227_BasicCalculatorII.ipynb</t>
-        </is>
-      </c>
-      <c r="F59" s="8" t="n">
-        <v>7</v>
-      </c>
       <c r="G59" s="3" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>Linked List</t>
         </is>
       </c>
       <c r="H59" s="3" t="inlineStr">
         <is>
-          <t>String</t>
-        </is>
-      </c>
-      <c r="I59" s="3" t="inlineStr">
-        <is>
-          <t>Math</t>
-        </is>
-      </c>
+          <t>Recursion</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="n"/>
       <c r="J59" s="3" t="n"/>
       <c r="K59" s="3" t="n"/>
     </row>
     <row r="60" hidden="1" ht="15.95" customHeight="1">
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>LC0238</t>
+          <t>LC0209</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>238</t>
+          <t>209</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
         <is>
-          <t>000027.LC0238.product-of-array-except-self.py</t>
+          <t>00018_LeetCode209_MinimumSizeSubarraySum.ipynb</t>
         </is>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000027.LC0238.product-of-array-except-self.py</t>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00018_LeetCode209_MinimumSizeSubarraySum.ipynb</t>
         </is>
       </c>
       <c r="F60" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G60" s="3" t="inlineStr">
         <is>
+          <t>Sliding Window</t>
+        </is>
+      </c>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
           <t>Array</t>
         </is>
       </c>
-      <c r="H60" s="3" t="inlineStr">
-        <is>
-          <t>Prefix Sum</t>
-        </is>
-      </c>
       <c r="I60" s="3" t="inlineStr">
         <is>
-          <t>Suffix Product</t>
+          <t>Two Pointers</t>
         </is>
       </c>
       <c r="J60" s="3" t="n"/>
       <c r="K60" s="3" t="n"/>
     </row>
     <row r="61" hidden="1" ht="15.95" customHeight="1">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>LC0238</t>
+          <t>LC0217</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>238</t>
+          <t>217</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
         <is>
-          <t>000028.LC0238.product-array-o1-space.py</t>
+          <t>00014_LeetCode217_ContainsDuplicate.ipynb</t>
         </is>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000028.LC0238.product-array-o1-space.py</t>
-        </is>
-      </c>
-      <c r="F61" s="5" t="n">
-        <v>6</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00014_LeetCode217_ContainsDuplicate.ipynb</t>
+        </is>
+      </c>
+      <c r="F61" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="G61" s="3" t="inlineStr">
         <is>
@@ -3129,36 +3143,37 @@
       </c>
       <c r="H61" s="3" t="inlineStr">
         <is>
-          <t>Prefix Sum</t>
-        </is>
-      </c>
-      <c r="I61" s="3" t="inlineStr">
-        <is>
-          <t>Suffix Product</t>
-        </is>
-      </c>
+          <t>Hash Set</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="n"/>
       <c r="J61" s="3" t="n"/>
       <c r="K61" s="3" t="n"/>
     </row>
-    <row r="62" ht="15.95" customHeight="1">
+    <row r="62" hidden="1" ht="15.95" customHeight="1">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>LC0242</t>
+          <t>LC0226</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>242</t>
+          <t>226</t>
         </is>
       </c>
       <c r="D62" s="3" t="inlineStr">
         <is>
-          <t>000026.LC0242.valid-anagram.redo.py</t>
+          <t>000022.LC0226.invert-binary-tree.py</t>
         </is>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000026.LC0242.valid-anagram.redo.py</t>
+          <t>C:\DataMajor\practice\000022.LC0226.invert-binary-tree.py</t>
         </is>
       </c>
       <c r="F62" s="4" t="n">
@@ -3166,91 +3181,87 @@
       </c>
       <c r="G62" s="3" t="inlineStr">
         <is>
-          <t>Hash Table</t>
+          <t>Tree</t>
         </is>
       </c>
       <c r="H62" s="3" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>Depth-First Search</t>
         </is>
       </c>
       <c r="I62" s="3" t="inlineStr">
         <is>
-          <t>Sorting</t>
-        </is>
-      </c>
-      <c r="J62" s="3" t="inlineStr">
-        <is>
-          <t>Sorting</t>
-        </is>
-      </c>
+          <t>Binary Tree</t>
+        </is>
+      </c>
+      <c r="J62" s="3" t="n"/>
       <c r="K62" s="3" t="n"/>
     </row>
     <row r="63" hidden="1" ht="15.95" customHeight="1">
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>LC0347</t>
+          <t>LC0227</t>
         </is>
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>347</t>
+          <t>227</t>
         </is>
       </c>
       <c r="D63" s="3" t="inlineStr">
         <is>
-          <t>00043_LeetCode347_TopKFrequentElements.ipynb</t>
+          <t>00042_LeetCode227_BasicCalculatorII.ipynb</t>
         </is>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00043_LeetCode347_TopKFrequentElements.ipynb</t>
-        </is>
-      </c>
-      <c r="F63" s="5" t="n">
-        <v>5</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00042_LeetCode227_BasicCalculatorII.ipynb</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="n">
+        <v>7</v>
       </c>
       <c r="G63" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Stack</t>
         </is>
       </c>
       <c r="H63" s="3" t="inlineStr">
         <is>
-          <t>Heap</t>
+          <t>String</t>
         </is>
       </c>
       <c r="I63" s="3" t="inlineStr">
         <is>
-          <t>Bucket Sort</t>
+          <t>Math</t>
         </is>
       </c>
       <c r="J63" s="3" t="n"/>
       <c r="K63" s="3" t="n"/>
     </row>
-    <row r="64" ht="15.95" customHeight="1">
+    <row r="64" hidden="1" ht="15.95" customHeight="1">
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>LC0378</t>
+          <t>LC0238</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>378</t>
+          <t>238</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
         <is>
-          <t>000002.LC0378.first-unique-char.py</t>
+          <t>000027.LC0238.product-of-array-except-self.py</t>
         </is>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000002.LC0378.first-unique-char.py</t>
-        </is>
-      </c>
-      <c r="F64" s="4" t="n">
-        <v>2</v>
+          <t>C:\DataMajor\practice\000027.LC0238.product-of-array-except-self.py</t>
+        </is>
+      </c>
+      <c r="F64" s="5" t="n">
+        <v>6</v>
       </c>
       <c r="G64" s="3" t="inlineStr">
         <is>
@@ -3259,230 +3270,241 @@
       </c>
       <c r="H64" s="3" t="inlineStr">
         <is>
-          <t>Binary Search</t>
+          <t>Prefix Sum</t>
         </is>
       </c>
       <c r="I64" s="3" t="inlineStr">
         <is>
-          <t>Matrix</t>
+          <t>Suffix Product</t>
         </is>
       </c>
       <c r="J64" s="3" t="n"/>
       <c r="K64" s="3" t="n"/>
     </row>
-    <row r="65" ht="15.95" customHeight="1">
+    <row r="65" hidden="1" ht="15.95" customHeight="1">
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>LC0387</t>
+          <t>LC0238</t>
         </is>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>387</t>
+          <t>238</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
         <is>
-          <t>000017.LC0387.first-unique-char.redo.py</t>
+          <t>000028.LC0238.product-array-o1-space.py</t>
         </is>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000017.LC0387.first-unique-char.redo.py</t>
-        </is>
-      </c>
-      <c r="F65" s="4" t="n">
-        <v>2</v>
+          <t>C:\DataMajor\practice\000028.LC0238.product-array-o1-space.py</t>
+        </is>
+      </c>
+      <c r="F65" s="5" t="n">
+        <v>6</v>
       </c>
       <c r="G65" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H65" s="3" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>Prefix Sum</t>
         </is>
       </c>
       <c r="I65" s="3" t="inlineStr">
         <is>
-          <t>Queue</t>
+          <t>Suffix Product</t>
         </is>
       </c>
       <c r="J65" s="3" t="n"/>
       <c r="K65" s="3" t="n"/>
     </row>
     <row r="66" hidden="1" ht="15.95" customHeight="1">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>LC0424</t>
+          <t>LC0242</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>424</t>
+          <t>242</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
         <is>
-          <t>00020_LeetCode424_LongestRepeatingCharacterReplacement.ipynb</t>
+          <t>000026.LC0242.valid-anagram.redo.py</t>
         </is>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00020_LeetCode424_LongestRepeatingCharacterReplacement.ipynb</t>
-        </is>
-      </c>
-      <c r="F66" s="5" t="n">
-        <v>6</v>
+          <t>C:\DataMajor\practice\000026.LC0242.valid-anagram.redo.py</t>
+        </is>
+      </c>
+      <c r="F66" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="G66" s="3" t="inlineStr">
         <is>
-          <t>Sliding Window</t>
+          <t>Hash Table</t>
         </is>
       </c>
       <c r="H66" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>String</t>
         </is>
       </c>
       <c r="I66" s="3" t="inlineStr">
         <is>
-          <t>String</t>
-        </is>
-      </c>
-      <c r="J66" s="3" t="inlineStr">
-        <is>
-          <t>Two Pointers</t>
-        </is>
-      </c>
+          <t>Sorting</t>
+        </is>
+      </c>
+      <c r="J66" s="3" t="n"/>
       <c r="K66" s="3" t="n"/>
     </row>
     <row r="67" hidden="1" ht="15.95" customHeight="1">
       <c r="B67" s="2" t="inlineStr">
         <is>
-          <t>LC0424</t>
+          <t>LC0347</t>
         </is>
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>424</t>
+          <t>347</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
         <is>
-          <t>000034.LC0424.longest-repeating-char-replacement.py</t>
+          <t>00043_LeetCode347_TopKFrequentElements.ipynb</t>
         </is>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000034.LC0424.longest-repeating-char-replacement.py</t>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00043_LeetCode347_TopKFrequentElements.ipynb</t>
         </is>
       </c>
       <c r="F67" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G67" s="3" t="inlineStr">
         <is>
-          <t>Sliding Window</t>
+          <t>Hash Map</t>
         </is>
       </c>
       <c r="H67" s="3" t="inlineStr">
         <is>
+          <t>Heap</t>
+        </is>
+      </c>
+      <c r="I67" s="3" t="inlineStr">
+        <is>
+          <t>Bucket Sort</t>
+        </is>
+      </c>
+      <c r="J67" s="3" t="n"/>
+      <c r="K67" s="3" t="n"/>
+    </row>
+    <row r="68" hidden="1" ht="15.95" customHeight="1">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
+        <is>
+          <t>LC0378</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>378</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="inlineStr">
+        <is>
+          <t>000002.LC0378.first-unique-char.py</t>
+        </is>
+      </c>
+      <c r="E68" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\000002.LC0378.first-unique-char.py</t>
+        </is>
+      </c>
+      <c r="F68" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G68" s="3" t="inlineStr">
+        <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="H68" s="3" t="inlineStr">
+        <is>
+          <t>Binary Search</t>
+        </is>
+      </c>
+      <c r="I68" s="3" t="inlineStr">
+        <is>
+          <t>Matrix</t>
+        </is>
+      </c>
+      <c r="J68" s="3" t="inlineStr">
+        <is>
+          <t>Heap (Priority Queue)</t>
+        </is>
+      </c>
+      <c r="K68" s="3" t="n"/>
+    </row>
+    <row r="69" hidden="1" ht="15.95" customHeight="1">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B69" s="2" t="inlineStr">
+        <is>
+          <t>LC0387</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="inlineStr">
+        <is>
+          <t>387</t>
+        </is>
+      </c>
+      <c r="D69" s="3" t="inlineStr">
+        <is>
+          <t>000017.LC0387.first-unique-char.redo.py</t>
+        </is>
+      </c>
+      <c r="E69" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\000017.LC0387.first-unique-char.redo.py</t>
+        </is>
+      </c>
+      <c r="F69" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G69" s="3" t="inlineStr">
+        <is>
           <t>Hash Map</t>
         </is>
       </c>
-      <c r="I67" s="3" t="inlineStr">
+      <c r="H69" s="3" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="J67" s="3" t="inlineStr">
-        <is>
-          <t>Two Pointers</t>
-        </is>
-      </c>
-      <c r="K67" s="3" t="n"/>
-    </row>
-    <row r="68" hidden="1" ht="15.95" customHeight="1">
-      <c r="B68" s="2" t="inlineStr">
-        <is>
-          <t>LC0438</t>
-        </is>
-      </c>
-      <c r="C68" s="2" t="inlineStr">
-        <is>
-          <t>438</t>
-        </is>
-      </c>
-      <c r="D68" s="3" t="inlineStr">
-        <is>
-          <t>00044_LeetCode438_FindAllAnagramsInAString.ipynb</t>
-        </is>
-      </c>
-      <c r="E68" s="3" t="inlineStr">
-        <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00044_LeetCode438_FindAllAnagramsInAString.ipynb</t>
-        </is>
-      </c>
-      <c r="F68" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G68" s="3" t="inlineStr">
-        <is>
-          <t>Sliding Window</t>
-        </is>
-      </c>
-      <c r="H68" s="3" t="inlineStr">
-        <is>
-          <t>Hash Map</t>
-        </is>
-      </c>
-      <c r="I68" s="3" t="inlineStr">
-        <is>
-          <t>String</t>
-        </is>
-      </c>
-      <c r="J68" s="3" t="n"/>
-      <c r="K68" s="3" t="n"/>
-    </row>
-    <row r="69" hidden="1" ht="15.95" customHeight="1">
-      <c r="B69" s="2" t="inlineStr">
-        <is>
-          <t>LC0523</t>
-        </is>
-      </c>
-      <c r="C69" s="2" t="inlineStr">
-        <is>
-          <t>523</t>
-        </is>
-      </c>
-      <c r="D69" s="3" t="inlineStr">
-        <is>
-          <t>00045_LeetCode523_ContinuousSubarraySum.ipynb</t>
-        </is>
-      </c>
-      <c r="E69" s="3" t="inlineStr">
-        <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00045_LeetCode523_ContinuousSubarraySum.ipynb</t>
-        </is>
-      </c>
-      <c r="F69" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G69" s="3" t="inlineStr">
-        <is>
-          <t>Hash Map</t>
-        </is>
-      </c>
-      <c r="H69" s="3" t="inlineStr">
-        <is>
-          <t>Prefix Sum</t>
-        </is>
-      </c>
       <c r="I69" s="3" t="inlineStr">
         <is>
-          <t>Math</t>
+          <t>Queue</t>
         </is>
       </c>
       <c r="J69" s="3" t="n"/>
@@ -3491,106 +3513,114 @@
     <row r="70" hidden="1" ht="15.95" customHeight="1">
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>LC0525</t>
+          <t>LC0424</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>525</t>
+          <t>424</t>
         </is>
       </c>
       <c r="D70" s="3" t="inlineStr">
         <is>
-          <t>00016_LeetCode525_ContiguousArray.ipynb</t>
+          <t>00020_LeetCode424_LongestRepeatingCharacterReplacement.ipynb</t>
         </is>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00016_LeetCode525_ContiguousArray.ipynb</t>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00020_LeetCode424_LongestRepeatingCharacterReplacement.ipynb</t>
         </is>
       </c>
       <c r="F70" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G70" s="3" t="inlineStr">
         <is>
+          <t>Sliding Window</t>
+        </is>
+      </c>
+      <c r="H70" s="3" t="inlineStr">
+        <is>
           <t>Hash Map</t>
         </is>
       </c>
-      <c r="H70" s="3" t="inlineStr">
-        <is>
-          <t>Prefix Sum</t>
-        </is>
-      </c>
       <c r="I70" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
-        </is>
-      </c>
-      <c r="J70" s="3" t="n"/>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="J70" s="3" t="inlineStr">
+        <is>
+          <t>Two Pointers</t>
+        </is>
+      </c>
       <c r="K70" s="3" t="n"/>
     </row>
     <row r="71" hidden="1" ht="15.95" customHeight="1">
       <c r="B71" s="2" t="inlineStr">
         <is>
-          <t>LC0560</t>
+          <t>LC0424</t>
         </is>
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>560</t>
+          <t>424</t>
         </is>
       </c>
       <c r="D71" s="3" t="inlineStr">
         <is>
-          <t>00003_LeetCode560_BruteForce_Teaching.py</t>
+          <t>000034.LC0424.longest-repeating-char-replacement.py</t>
         </is>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Sean_Practice\00003_LeetCode560_BruteForce_Teaching.py</t>
+          <t>C:\DataMajor\practice\000034.LC0424.longest-repeating-char-replacement.py</t>
         </is>
       </c>
       <c r="F71" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G71" s="3" t="inlineStr">
         <is>
+          <t>Sliding Window</t>
+        </is>
+      </c>
+      <c r="H71" s="3" t="inlineStr">
+        <is>
           <t>Hash Map</t>
         </is>
       </c>
-      <c r="H71" s="3" t="inlineStr">
-        <is>
-          <t>Prefix Sum</t>
-        </is>
-      </c>
       <c r="I71" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
-        </is>
-      </c>
-      <c r="J71" s="3" t="n"/>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="J71" s="3" t="inlineStr">
+        <is>
+          <t>Two Pointers</t>
+        </is>
+      </c>
       <c r="K71" s="3" t="n"/>
     </row>
     <row r="72" hidden="1" ht="15.95" customHeight="1">
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>LC0560</t>
+          <t>LC0438</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>560</t>
+          <t>438</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
         <is>
-          <t>00011.LeetCode560.SubArryaySumK.ipynb</t>
+          <t>00044_LeetCode438_FindAllAnagramsInAString.ipynb</t>
         </is>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00011.LeetCode560.SubArryaySumK.ipynb</t>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00044_LeetCode438_FindAllAnagramsInAString.ipynb</t>
         </is>
       </c>
       <c r="F72" s="5" t="n">
@@ -3598,17 +3628,17 @@
       </c>
       <c r="G72" s="3" t="inlineStr">
         <is>
+          <t>Sliding Window</t>
+        </is>
+      </c>
+      <c r="H72" s="3" t="inlineStr">
+        <is>
           <t>Hash Map</t>
         </is>
       </c>
-      <c r="H72" s="3" t="inlineStr">
-        <is>
-          <t>Prefix Sum</t>
-        </is>
-      </c>
       <c r="I72" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
+          <t>String</t>
         </is>
       </c>
       <c r="J72" s="3" t="n"/>
@@ -3617,26 +3647,26 @@
     <row r="73" hidden="1" ht="15.95" customHeight="1">
       <c r="B73" s="2" t="inlineStr">
         <is>
-          <t>LC0560</t>
+          <t>LC0523</t>
         </is>
       </c>
       <c r="C73" s="2" t="inlineStr">
         <is>
-          <t>560</t>
+          <t>523</t>
         </is>
       </c>
       <c r="D73" s="3" t="inlineStr">
         <is>
-          <t>00004_LeetCode560_BruteForce_ListTests.py</t>
+          <t>00045_LeetCode523_ContinuousSubarraySum.ipynb</t>
         </is>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Sean_Practice\00004_LeetCode560_BruteForce_ListTests.py</t>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00045_LeetCode523_ContinuousSubarraySum.ipynb</t>
         </is>
       </c>
       <c r="F73" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G73" s="3" t="inlineStr">
         <is>
@@ -3650,7 +3680,7 @@
       </c>
       <c r="I73" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
+          <t>Math</t>
         </is>
       </c>
       <c r="J73" s="3" t="n"/>
@@ -3659,22 +3689,22 @@
     <row r="74" hidden="1" ht="15.95" customHeight="1">
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>LC0567</t>
+          <t>LC0525</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>567</t>
+          <t>525</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
         <is>
-          <t>00021_LeetCode567_PermutationInString.ipynb</t>
+          <t>00016_LeetCode525_ContiguousArray.ipynb</t>
         </is>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00021_LeetCode567_PermutationInString.ipynb</t>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00016_LeetCode525_ContiguousArray.ipynb</t>
         </is>
       </c>
       <c r="F74" s="5" t="n">
@@ -3682,17 +3712,17 @@
       </c>
       <c r="G74" s="3" t="inlineStr">
         <is>
-          <t>Sliding Window</t>
+          <t>Hash Map</t>
         </is>
       </c>
       <c r="H74" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Prefix Sum</t>
         </is>
       </c>
       <c r="I74" s="3" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="J74" s="3" t="n"/>
@@ -3701,193 +3731,190 @@
     <row r="75" hidden="1" ht="15.95" customHeight="1">
       <c r="B75" s="2" t="inlineStr">
         <is>
-          <t>LC0674</t>
+          <t>LC0560</t>
         </is>
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>674</t>
+          <t>560</t>
         </is>
       </c>
       <c r="D75" s="3" t="inlineStr">
         <is>
-          <t>5LeetCode674.LongestIncreasingSubSequence.ipynb</t>
+          <t>00003_LeetCode560_BruteForce_Teaching.py</t>
         </is>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\5LeetCode674.LongestIncreasingSubSequence.ipynb</t>
-        </is>
-      </c>
-      <c r="F75" s="6" t="n">
-        <v>4</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Sean_Practice\00003_LeetCode560_BruteForce_Teaching.py</t>
+        </is>
+      </c>
+      <c r="F75" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G75" s="3" t="inlineStr">
         <is>
-          <t>Dynamic Programming</t>
+          <t>Hash Map</t>
         </is>
       </c>
       <c r="H75" s="3" t="inlineStr">
         <is>
+          <t>Prefix Sum</t>
+        </is>
+      </c>
+      <c r="I75" s="3" t="inlineStr">
+        <is>
           <t>Array</t>
-        </is>
-      </c>
-      <c r="I75" s="3" t="inlineStr">
-        <is>
-          <t>Greedy</t>
         </is>
       </c>
       <c r="J75" s="3" t="n"/>
       <c r="K75" s="3" t="n"/>
     </row>
     <row r="76" hidden="1" ht="15.95" customHeight="1">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>LC0704</t>
+          <t>LC0560</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>704</t>
+          <t>560</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
         <is>
-          <t>000008.LC0704.binary-search.py</t>
+          <t>00011.LeetCode560.SubArryaySumK.ipynb</t>
         </is>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000008.LC0704.binary-search.py</t>
-        </is>
-      </c>
-      <c r="F76" s="4" t="n">
-        <v>3</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00011.LeetCode560.SubArryaySumK.ipynb</t>
+        </is>
+      </c>
+      <c r="F76" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G76" s="3" t="inlineStr">
         <is>
-          <t>Binary Search</t>
+          <t>Hash Map</t>
         </is>
       </c>
       <c r="H76" s="3" t="inlineStr">
         <is>
+          <t>Prefix Sum</t>
+        </is>
+      </c>
+      <c r="I76" s="3" t="inlineStr">
+        <is>
           <t>Array</t>
         </is>
       </c>
-      <c r="I76" s="3" t="n"/>
       <c r="J76" s="3" t="n"/>
       <c r="K76" s="3" t="n"/>
     </row>
     <row r="77" hidden="1" ht="15.95" customHeight="1">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="B77" s="2" t="inlineStr">
         <is>
-          <t>LC0704</t>
+          <t>LC0560</t>
         </is>
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>704</t>
+          <t>560</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
         <is>
-          <t>000020.LC0704.binary-search.redo.py</t>
+          <t>00004_LeetCode560_BruteForce_ListTests.py</t>
         </is>
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000020.LC0704.binary-search.redo.py</t>
-        </is>
-      </c>
-      <c r="F77" s="4" t="n">
-        <v>3</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Sean_Practice\00004_LeetCode560_BruteForce_ListTests.py</t>
+        </is>
+      </c>
+      <c r="F77" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G77" s="3" t="inlineStr">
         <is>
-          <t>Binary Search</t>
+          <t>Hash Map</t>
         </is>
       </c>
       <c r="H77" s="3" t="inlineStr">
         <is>
+          <t>Prefix Sum</t>
+        </is>
+      </c>
+      <c r="I77" s="3" t="inlineStr">
+        <is>
           <t>Array</t>
         </is>
       </c>
-      <c r="I77" s="3" t="n"/>
       <c r="J77" s="3" t="n"/>
       <c r="K77" s="3" t="n"/>
     </row>
     <row r="78" hidden="1" ht="15.95" customHeight="1">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>LC0704</t>
+          <t>LC0567</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>704</t>
+          <t>567</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
         <is>
-          <t>00704_LeetCode704_BinarySearch.ipynb</t>
+          <t>00021_LeetCode567_PermutationInString.ipynb</t>
         </is>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00704_LeetCode704_BinarySearch.ipynb</t>
-        </is>
-      </c>
-      <c r="F78" s="4" t="n">
-        <v>3</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00021_LeetCode567_PermutationInString.ipynb</t>
+        </is>
+      </c>
+      <c r="F78" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G78" s="3" t="inlineStr">
         <is>
-          <t>Binary Search</t>
+          <t>Sliding Window</t>
         </is>
       </c>
       <c r="H78" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
-        </is>
-      </c>
-      <c r="I78" s="3" t="n"/>
+          <t>Hash Map</t>
+        </is>
+      </c>
+      <c r="I78" s="3" t="inlineStr">
+        <is>
+          <t>String</t>
+        </is>
+      </c>
       <c r="J78" s="3" t="n"/>
       <c r="K78" s="3" t="n"/>
     </row>
     <row r="79" hidden="1" ht="15.95" customHeight="1">
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t>LC0937</t>
+          <t>LC0674</t>
         </is>
       </c>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>937</t>
+          <t>674</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
         <is>
-          <t>00015_LeetCode937_ReorderLogFiles.ipynb</t>
+          <t>5LeetCode674.LongestIncreasingSubSequence.ipynb</t>
         </is>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00015_LeetCode937_ReorderLogFiles.ipynb</t>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\5LeetCode674.LongestIncreasingSubSequence.ipynb</t>
         </is>
       </c>
       <c r="F79" s="6" t="n">
@@ -3895,133 +3922,140 @@
       </c>
       <c r="G79" s="3" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>Dynamic Programming</t>
         </is>
       </c>
       <c r="H79" s="3" t="inlineStr">
         <is>
-          <t>Sorting</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="I79" s="3" t="inlineStr">
         <is>
-          <t>Custom Sort</t>
+          <t>Greedy</t>
         </is>
       </c>
       <c r="J79" s="3" t="n"/>
       <c r="K79" s="3" t="n"/>
     </row>
     <row r="80" hidden="1" ht="15.95" customHeight="1">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>LC0937</t>
+          <t>LC0704</t>
         </is>
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>937</t>
+          <t>704</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
         <is>
-          <t>00010.LeetCode937.Reorder Data in Log Files.ipynb</t>
+          <t>000008.LC0704.binary-search.py</t>
         </is>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00010.LeetCode937.Reorder Data in Log Files.ipynb</t>
-        </is>
-      </c>
-      <c r="F80" s="6" t="n">
-        <v>4</v>
+          <t>C:\DataMajor\practice\000008.LC0704.binary-search.py</t>
+        </is>
+      </c>
+      <c r="F80" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="G80" s="3" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>Binary Search</t>
         </is>
       </c>
       <c r="H80" s="3" t="inlineStr">
         <is>
-          <t>Sorting</t>
-        </is>
-      </c>
-      <c r="I80" s="3" t="inlineStr">
-        <is>
-          <t>Custom Sort</t>
-        </is>
-      </c>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="I80" s="3" t="n"/>
       <c r="J80" s="3" t="n"/>
       <c r="K80" s="3" t="n"/>
     </row>
     <row r="81" hidden="1" ht="15.95" customHeight="1">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B81" s="2" t="inlineStr">
         <is>
-          <t>LC0974</t>
+          <t>LC0704</t>
         </is>
       </c>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t>974</t>
+          <t>704</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
         <is>
-          <t>00012.LeetCode974.SubArraySumsDivisable974.ipynb</t>
+          <t>000020.LC0704.binary-search.redo.py</t>
         </is>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00012.LeetCode974.SubArraySumsDivisable974.ipynb</t>
-        </is>
-      </c>
-      <c r="F81" s="5" t="n">
-        <v>6</v>
+          <t>C:\DataMajor\practice\000020.LC0704.binary-search.redo.py</t>
+        </is>
+      </c>
+      <c r="F81" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="G81" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Binary Search</t>
         </is>
       </c>
       <c r="H81" s="3" t="inlineStr">
         <is>
-          <t>Prefix Sum</t>
-        </is>
-      </c>
-      <c r="I81" s="3" t="inlineStr">
-        <is>
-          <t>Math</t>
-        </is>
-      </c>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="I81" s="3" t="n"/>
       <c r="J81" s="3" t="n"/>
       <c r="K81" s="3" t="n"/>
     </row>
     <row r="82" hidden="1" ht="15.95" customHeight="1">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>LC1004</t>
+          <t>LC0704</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>1004</t>
+          <t>704</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
         <is>
-          <t>00023_LeetCode1004_MaxConsecutiveOnesIII.ipynb</t>
+          <t>00704_LeetCode704_BinarySearch.ipynb</t>
         </is>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00023_LeetCode1004_MaxConsecutiveOnesIII.ipynb</t>
-        </is>
-      </c>
-      <c r="F82" s="5" t="n">
-        <v>5</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00704_LeetCode704_BinarySearch.ipynb</t>
+        </is>
+      </c>
+      <c r="F82" s="4" t="n">
+        <v>3</v>
       </c>
       <c r="G82" s="3" t="inlineStr">
         <is>
-          <t>Sliding Window</t>
+          <t>Binary Search</t>
         </is>
       </c>
       <c r="H82" s="3" t="inlineStr">
@@ -4029,79 +4063,71 @@
           <t>Array</t>
         </is>
       </c>
-      <c r="I82" s="3" t="inlineStr">
-        <is>
-          <t>Two Pointers</t>
-        </is>
-      </c>
+      <c r="I82" s="3" t="n"/>
       <c r="J82" s="3" t="n"/>
       <c r="K82" s="3" t="n"/>
     </row>
     <row r="83" hidden="1" ht="15.95" customHeight="1">
       <c r="B83" s="2" t="inlineStr">
         <is>
-          <t>LC1861</t>
+          <t>LC0937</t>
         </is>
       </c>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>1861</t>
+          <t>937</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
         <is>
-          <t>00046_LeetCode1861_RotatingTheBox.ipynb</t>
+          <t>00015_LeetCode937_ReorderLogFiles.ipynb</t>
         </is>
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00046_LeetCode1861_RotatingTheBox.ipynb</t>
-        </is>
-      </c>
-      <c r="F83" s="5" t="n">
-        <v>6</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00015_LeetCode937_ReorderLogFiles.ipynb</t>
+        </is>
+      </c>
+      <c r="F83" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="G83" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
+          <t>String</t>
         </is>
       </c>
       <c r="H83" s="3" t="inlineStr">
         <is>
-          <t>Matrix</t>
+          <t>Sorting</t>
         </is>
       </c>
       <c r="I83" s="3" t="inlineStr">
         <is>
-          <t>Two Pointers</t>
-        </is>
-      </c>
-      <c r="J83" s="3" t="inlineStr">
-        <is>
-          <t>Simulation</t>
-        </is>
-      </c>
+          <t>Custom Sort</t>
+        </is>
+      </c>
+      <c r="J83" s="3" t="n"/>
       <c r="K83" s="3" t="n"/>
     </row>
     <row r="84" hidden="1" ht="15.95" customHeight="1">
       <c r="B84" s="2" t="inlineStr">
         <is>
-          <t>LC2043</t>
+          <t>LC0937</t>
         </is>
       </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>2043</t>
+          <t>937</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
         <is>
-          <t>00017_LeetCode2043_SimpleBankSystem.ipynb</t>
+          <t>00010.LeetCode937.Reorder Data in Log Files.ipynb</t>
         </is>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00017_LeetCode2043_SimpleBankSystem.ipynb</t>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00010.LeetCode937.Reorder Data in Log Files.ipynb</t>
         </is>
       </c>
       <c r="F84" s="6" t="n">
@@ -4109,17 +4135,17 @@
       </c>
       <c r="G84" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
+          <t>String</t>
         </is>
       </c>
       <c r="H84" s="3" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>Sorting</t>
         </is>
       </c>
       <c r="I84" s="3" t="inlineStr">
         <is>
-          <t>Simulation</t>
+          <t>Custom Sort</t>
         </is>
       </c>
       <c r="J84" s="3" t="n"/>
@@ -4128,86 +4154,82 @@
     <row r="85" hidden="1" ht="15.95" customHeight="1">
       <c r="B85" s="2" t="inlineStr">
         <is>
-          <t>LC3045</t>
+          <t>LC0974</t>
         </is>
       </c>
       <c r="C85" s="2" t="inlineStr">
         <is>
-          <t>3045</t>
+          <t>974</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
         <is>
-          <t>00047_LeetCode3045_CountPrefixSuffixPairsII.ipynb</t>
+          <t>00012.LeetCode974.SubArraySumsDivisable974.ipynb</t>
         </is>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00047_LeetCode3045_CountPrefixSuffixPairsII.ipynb</t>
-        </is>
-      </c>
-      <c r="F85" s="8" t="n">
-        <v>8</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00012.LeetCode974.SubArraySumsDivisable974.ipynb</t>
+        </is>
+      </c>
+      <c r="F85" s="5" t="n">
+        <v>6</v>
       </c>
       <c r="G85" s="3" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>Hash Map</t>
         </is>
       </c>
       <c r="H85" s="3" t="inlineStr">
         <is>
-          <t>Hashing</t>
+          <t>Prefix Sum</t>
         </is>
       </c>
       <c r="I85" s="3" t="inlineStr">
         <is>
-          <t>Z-Algorithm</t>
-        </is>
-      </c>
-      <c r="J85" s="3" t="inlineStr">
-        <is>
-          <t>Trie</t>
-        </is>
-      </c>
+          <t>Math</t>
+        </is>
+      </c>
+      <c r="J85" s="3" t="n"/>
       <c r="K85" s="3" t="n"/>
     </row>
     <row r="86" hidden="1" ht="15.95" customHeight="1">
       <c r="B86" s="2" t="inlineStr">
         <is>
-          <t>LC3161</t>
+          <t>LC1004</t>
         </is>
       </c>
       <c r="C86" s="2" t="inlineStr">
         <is>
-          <t>3161</t>
+          <t>1004</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
         <is>
-          <t>00048_LeetCode3161_BlockPlacementQueries.ipynb</t>
+          <t>00023_LeetCode1004_MaxConsecutiveOnesIII.ipynb</t>
         </is>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00048_LeetCode3161_BlockPlacementQueries.ipynb</t>
-        </is>
-      </c>
-      <c r="F86" s="7" t="n">
-        <v>9</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00023_LeetCode1004_MaxConsecutiveOnesIII.ipynb</t>
+        </is>
+      </c>
+      <c r="F86" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G86" s="3" t="inlineStr">
         <is>
-          <t>Binary Indexed Tree</t>
+          <t>Sliding Window</t>
         </is>
       </c>
       <c r="H86" s="3" t="inlineStr">
         <is>
-          <t>Segment Tree</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="I86" s="3" t="inlineStr">
         <is>
-          <t>Binary Search</t>
+          <t>Two Pointers</t>
         </is>
       </c>
       <c r="J86" s="3" t="n"/>
@@ -4216,82 +4238,86 @@
     <row r="87" hidden="1" ht="15.95" customHeight="1">
       <c r="B87" s="2" t="inlineStr">
         <is>
-          <t>LEC0020</t>
+          <t>LC1861</t>
         </is>
       </c>
       <c r="C87" s="2" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>1861</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
         <is>
-          <t>000005.LEC0020.valid-parentheses.py</t>
+          <t>00046_LeetCode1861_RotatingTheBox.ipynb</t>
         </is>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000005.LEC0020.valid-parentheses.py</t>
-        </is>
-      </c>
-      <c r="F87" s="6" t="n">
-        <v>3</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00046_LeetCode1861_RotatingTheBox.ipynb</t>
+        </is>
+      </c>
+      <c r="F87" s="5" t="n">
+        <v>6</v>
       </c>
       <c r="G87" s="3" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H87" s="3" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>Matrix</t>
         </is>
       </c>
       <c r="I87" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
-        </is>
-      </c>
-      <c r="J87" s="3" t="n"/>
+          <t>Two Pointers</t>
+        </is>
+      </c>
+      <c r="J87" s="3" t="inlineStr">
+        <is>
+          <t>Simulation</t>
+        </is>
+      </c>
       <c r="K87" s="3" t="n"/>
     </row>
     <row r="88" hidden="1" ht="15.95" customHeight="1">
       <c r="B88" s="2" t="inlineStr">
         <is>
-          <t>LEC0084</t>
+          <t>LC2043</t>
         </is>
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>2043</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
         <is>
-          <t>LEC84.ipynb</t>
+          <t>00017_LeetCode2043_SimpleBankSystem.ipynb</t>
         </is>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC84.ipynb</t>
-        </is>
-      </c>
-      <c r="F88" s="8" t="n">
-        <v>8</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00017_LeetCode2043_SimpleBankSystem.ipynb</t>
+        </is>
+      </c>
+      <c r="F88" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="G88" s="3" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H88" s="3" t="inlineStr">
         <is>
-          <t>Monotonic Stack</t>
+          <t>Design</t>
         </is>
       </c>
       <c r="I88" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
+          <t>Simulation</t>
         </is>
       </c>
       <c r="J88" s="3" t="n"/>
@@ -4300,45 +4326,45 @@
     <row r="89" hidden="1" ht="15.95" customHeight="1">
       <c r="B89" s="2" t="inlineStr">
         <is>
-          <t>LEC0200</t>
+          <t>LC3045</t>
         </is>
       </c>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>3045</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
         <is>
-          <t>LEC200_Dfs.py</t>
+          <t>00047_LeetCode3045_CountPrefixSuffixPairsII.ipynb</t>
         </is>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\playground\DSA\smallScripts\LEC200_Dfs.py</t>
-        </is>
-      </c>
-      <c r="F89" s="5" t="n">
-        <v>5</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00047_LeetCode3045_CountPrefixSuffixPairsII.ipynb</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="n">
+        <v>8</v>
       </c>
       <c r="G89" s="3" t="inlineStr">
         <is>
-          <t>DFS</t>
+          <t>String</t>
         </is>
       </c>
       <c r="H89" s="3" t="inlineStr">
         <is>
-          <t>BFS</t>
+          <t>Hashing</t>
         </is>
       </c>
       <c r="I89" s="3" t="inlineStr">
         <is>
-          <t>Matrix</t>
+          <t>Z-Algorithm</t>
         </is>
       </c>
       <c r="J89" s="3" t="inlineStr">
         <is>
-          <t>Union Find</t>
+          <t>Trie</t>
         </is>
       </c>
       <c r="K89" s="3" t="n"/>
@@ -4346,167 +4372,176 @@
     <row r="90" hidden="1" ht="15.95" customHeight="1">
       <c r="B90" s="2" t="inlineStr">
         <is>
-          <t>LEC0200</t>
+          <t>LC3161</t>
         </is>
       </c>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>3161</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
         <is>
-          <t>LEC200bfs.py</t>
+          <t>00048_LeetCode3161_BlockPlacementQueries.ipynb</t>
         </is>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\playground\DSA\smallScripts\LEC200bfs.py</t>
-        </is>
-      </c>
-      <c r="F90" s="5" t="n">
-        <v>5</v>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00048_LeetCode3161_BlockPlacementQueries.ipynb</t>
+        </is>
+      </c>
+      <c r="F90" s="7" t="n">
+        <v>9</v>
       </c>
       <c r="G90" s="3" t="inlineStr">
         <is>
-          <t>DFS</t>
+          <t>Binary Indexed Tree</t>
         </is>
       </c>
       <c r="H90" s="3" t="inlineStr">
         <is>
-          <t>BFS</t>
+          <t>Segment Tree</t>
         </is>
       </c>
       <c r="I90" s="3" t="inlineStr">
         <is>
-          <t>Matrix</t>
-        </is>
-      </c>
-      <c r="J90" s="3" t="inlineStr">
-        <is>
-          <t>Union Find</t>
-        </is>
-      </c>
+          <t>Binary Search</t>
+        </is>
+      </c>
+      <c r="J90" s="3" t="n"/>
       <c r="K90" s="3" t="n"/>
     </row>
     <row r="91" ht="15.95" customHeight="1">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B91" s="2" t="inlineStr">
         <is>
-          <t>LEC0206</t>
+          <t>LEC0020</t>
         </is>
       </c>
       <c r="C91" s="2" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
         <is>
-          <t>000036.LEC0206.reverse-linked-list.redo.py</t>
+          <t>000005.LEC0020.valid-parentheses.py</t>
         </is>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000036.LEC0206.reverse-linked-list.redo.py</t>
-        </is>
-      </c>
-      <c r="F91" s="4" t="n">
+          <t>C:\DataMajor\practice\000005.LEC0020.valid-parentheses.py</t>
+        </is>
+      </c>
+      <c r="F91" s="6" t="n">
         <v>1</v>
       </c>
       <c r="G91" s="3" t="inlineStr">
         <is>
-          <t>Linked List</t>
+          <t>String</t>
         </is>
       </c>
       <c r="H91" s="3" t="inlineStr">
         <is>
-          <t>Recursion</t>
-        </is>
-      </c>
-      <c r="I91" s="3" t="n"/>
+          <t>Stack</t>
+        </is>
+      </c>
+      <c r="I91" s="3" t="inlineStr">
+        <is>
+          <t>Hash Map</t>
+        </is>
+      </c>
       <c r="J91" s="3" t="n"/>
       <c r="K91" s="3" t="n"/>
     </row>
-    <row r="92" ht="15.95" customHeight="1">
+    <row r="92" hidden="1" ht="15.95" customHeight="1">
       <c r="B92" s="2" t="inlineStr">
         <is>
-          <t>LEC0206</t>
+          <t>LEC0084</t>
         </is>
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>84</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
         <is>
-          <t>000006.LEC0206.reverse-linked-list.py</t>
+          <t>LEC84.ipynb</t>
         </is>
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000006.LEC0206.reverse-linked-list.py</t>
-        </is>
-      </c>
-      <c r="F92" s="4" t="n">
-        <v>1</v>
+          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC84.ipynb</t>
+        </is>
+      </c>
+      <c r="F92" s="8" t="n">
+        <v>8</v>
       </c>
       <c r="G92" s="3" t="inlineStr">
         <is>
-          <t>Linked List</t>
+          <t>Stack</t>
         </is>
       </c>
       <c r="H92" s="3" t="inlineStr">
         <is>
-          <t>Recursion</t>
-        </is>
-      </c>
-      <c r="I92" s="3" t="n"/>
+          <t>Monotonic Stack</t>
+        </is>
+      </c>
+      <c r="I92" s="3" t="inlineStr">
+        <is>
+          <t>Array</t>
+        </is>
+      </c>
       <c r="J92" s="3" t="n"/>
       <c r="K92" s="3" t="n"/>
     </row>
-    <row r="93" ht="15.95" customHeight="1">
+    <row r="93" hidden="1" ht="15.95" customHeight="1">
       <c r="B93" s="2" t="inlineStr">
         <is>
-          <t>LEC0242</t>
+          <t>LEC0200</t>
         </is>
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
-          <t>242</t>
+          <t>200</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
         <is>
-          <t>000004.LEC0242.valid-anagram.py</t>
+          <t>LEC200_Dfs.py</t>
         </is>
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\practice\000004.LEC0242.valid-anagram.py</t>
-        </is>
-      </c>
-      <c r="F93" s="4" t="n">
-        <v>1</v>
+          <t>C:\DataMajor\playground\DSA\smallScripts\LEC200_Dfs.py</t>
+        </is>
+      </c>
+      <c r="F93" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G93" s="3" t="inlineStr">
         <is>
-          <t>Hash Table</t>
+          <t>DFS</t>
         </is>
       </c>
       <c r="H93" s="3" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>BFS</t>
         </is>
       </c>
       <c r="I93" s="3" t="inlineStr">
         <is>
-          <t>Sorting</t>
+          <t>Matrix</t>
         </is>
       </c>
       <c r="J93" s="3" t="inlineStr">
         <is>
-          <t>Sorting</t>
+          <t>Union Find</t>
         </is>
       </c>
       <c r="K93" s="3" t="n"/>
@@ -4514,194 +4549,209 @@
     <row r="94" hidden="1" ht="15.95" customHeight="1">
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>LEC0496</t>
+          <t>LEC0200</t>
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>496</t>
+          <t>200</t>
         </is>
       </c>
       <c r="D94" s="3" t="inlineStr">
         <is>
-          <t>LEC496.ipynb</t>
+          <t>LEC200bfs.py</t>
         </is>
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC496.ipynb</t>
-        </is>
-      </c>
-      <c r="F94" s="6" t="n">
-        <v>4</v>
+          <t>C:\DataMajor\playground\DSA\smallScripts\LEC200bfs.py</t>
+        </is>
+      </c>
+      <c r="F94" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="G94" s="3" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>DFS</t>
         </is>
       </c>
       <c r="H94" s="3" t="inlineStr">
         <is>
-          <t>Monotonic Stack</t>
+          <t>BFS</t>
         </is>
       </c>
       <c r="I94" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
-        </is>
-      </c>
-      <c r="J94" s="3" t="n"/>
+          <t>Matrix</t>
+        </is>
+      </c>
+      <c r="J94" s="3" t="inlineStr">
+        <is>
+          <t>Union Find</t>
+        </is>
+      </c>
       <c r="K94" s="3" t="n"/>
     </row>
     <row r="95" hidden="1" ht="15.95" customHeight="1">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B95" s="2" t="inlineStr">
         <is>
-          <t>LEC0503</t>
+          <t>LEC0206</t>
         </is>
       </c>
       <c r="C95" s="2" t="inlineStr">
         <is>
-          <t>503</t>
+          <t>206</t>
         </is>
       </c>
       <c r="D95" s="3" t="inlineStr">
         <is>
-          <t>LEC503.ipynb</t>
+          <t>000036.LEC0206.reverse-linked-list.redo.py</t>
         </is>
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC503.ipynb</t>
-        </is>
-      </c>
-      <c r="F95" s="5" t="n">
-        <v>5</v>
+          <t>C:\DataMajor\practice\000036.LEC0206.reverse-linked-list.redo.py</t>
+        </is>
+      </c>
+      <c r="F95" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="G95" s="3" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>Linked List</t>
         </is>
       </c>
       <c r="H95" s="3" t="inlineStr">
         <is>
-          <t>Monotonic Stack</t>
-        </is>
-      </c>
-      <c r="I95" s="3" t="inlineStr">
-        <is>
-          <t>Circular Array</t>
-        </is>
-      </c>
+          <t>Recursion</t>
+        </is>
+      </c>
+      <c r="I95" s="3" t="n"/>
       <c r="J95" s="3" t="n"/>
       <c r="K95" s="3" t="n"/>
     </row>
     <row r="96" hidden="1" ht="15.95" customHeight="1">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B96" s="2" t="inlineStr">
         <is>
-          <t>LEC0739</t>
+          <t>LEC0206</t>
         </is>
       </c>
       <c r="C96" s="2" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>206</t>
         </is>
       </c>
       <c r="D96" s="3" t="inlineStr">
         <is>
-          <t>LEC739.ipynb</t>
+          <t>000006.LEC0206.reverse-linked-list.py</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC739.ipynb</t>
-        </is>
-      </c>
-      <c r="F96" s="5" t="n">
-        <v>5</v>
+          <t>C:\DataMajor\practice\000006.LEC0206.reverse-linked-list.py</t>
+        </is>
+      </c>
+      <c r="F96" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="G96" s="3" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>Linked List</t>
         </is>
       </c>
       <c r="H96" s="3" t="inlineStr">
         <is>
-          <t>Monotonic Stack</t>
-        </is>
-      </c>
-      <c r="I96" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
-        </is>
-      </c>
+          <t>Recursion</t>
+        </is>
+      </c>
+      <c r="I96" s="3" t="n"/>
       <c r="J96" s="3" t="n"/>
       <c r="K96" s="3" t="n"/>
     </row>
     <row r="97" hidden="1" ht="15.95" customHeight="1">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B97" s="2" t="inlineStr">
         <is>
-          <t>LEC0739</t>
+          <t>LEC0242</t>
         </is>
       </c>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>242</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
         <is>
-          <t>lec739.ipynb</t>
+          <t>000004.LEC0242.valid-anagram.py</t>
         </is>
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\playground\scratch\lec739.ipynb</t>
-        </is>
-      </c>
-      <c r="F97" s="5" t="n">
-        <v>5</v>
+          <t>C:\DataMajor\practice\000004.LEC0242.valid-anagram.py</t>
+        </is>
+      </c>
+      <c r="F97" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="G97" s="3" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>Hash Table</t>
         </is>
       </c>
       <c r="H97" s="3" t="inlineStr">
         <is>
-          <t>Monotonic Stack</t>
+          <t>String</t>
         </is>
       </c>
       <c r="I97" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
-        </is>
-      </c>
-      <c r="J97" s="3" t="n"/>
+          <t>Sorting</t>
+        </is>
+      </c>
+      <c r="J97" s="3" t="inlineStr">
+        <is>
+          <t>Sorting</t>
+        </is>
+      </c>
       <c r="K97" s="3" t="n"/>
     </row>
     <row r="98" hidden="1" ht="15.95" customHeight="1">
       <c r="B98" s="2" t="inlineStr">
         <is>
-          <t>LEC0901</t>
+          <t>LEC0496</t>
         </is>
       </c>
       <c r="C98" s="2" t="inlineStr">
         <is>
-          <t>901</t>
+          <t>496</t>
         </is>
       </c>
       <c r="D98" s="3" t="inlineStr">
         <is>
-          <t>LEC901.ipynb</t>
+          <t>LEC496.ipynb</t>
         </is>
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC901.ipynb</t>
-        </is>
-      </c>
-      <c r="F98" s="5" t="n">
-        <v>6</v>
+          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC496.ipynb</t>
+        </is>
+      </c>
+      <c r="F98" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="G98" s="3" t="inlineStr">
         <is>
@@ -4715,20 +4765,397 @@
       </c>
       <c r="I98" s="3" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>Hash Map</t>
         </is>
       </c>
       <c r="J98" s="3" t="n"/>
       <c r="K98" s="3" t="n"/>
     </row>
+    <row r="99" hidden="1" ht="15.95" customHeight="1">
+      <c r="B99" s="2" t="inlineStr">
+        <is>
+          <t>LEC0503</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="inlineStr">
+        <is>
+          <t>503</t>
+        </is>
+      </c>
+      <c r="D99" s="3" t="inlineStr">
+        <is>
+          <t>LEC503.ipynb</t>
+        </is>
+      </c>
+      <c r="E99" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC503.ipynb</t>
+        </is>
+      </c>
+      <c r="F99" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G99" s="3" t="inlineStr">
+        <is>
+          <t>Stack</t>
+        </is>
+      </c>
+      <c r="H99" s="3" t="inlineStr">
+        <is>
+          <t>Monotonic Stack</t>
+        </is>
+      </c>
+      <c r="I99" s="3" t="inlineStr">
+        <is>
+          <t>Circular Array</t>
+        </is>
+      </c>
+      <c r="J99" s="3" t="n"/>
+      <c r="K99" s="3" t="n"/>
+    </row>
+    <row r="100" hidden="1" ht="15.95" customHeight="1">
+      <c r="B100" s="2" t="inlineStr">
+        <is>
+          <t>LEC0739</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="inlineStr">
+        <is>
+          <t>739</t>
+        </is>
+      </c>
+      <c r="D100" s="3" t="inlineStr">
+        <is>
+          <t>LEC739.ipynb</t>
+        </is>
+      </c>
+      <c r="E100" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC739.ipynb</t>
+        </is>
+      </c>
+      <c r="F100" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G100" s="3" t="inlineStr">
+        <is>
+          <t>Stack</t>
+        </is>
+      </c>
+      <c r="H100" s="3" t="inlineStr">
+        <is>
+          <t>Monotonic Stack</t>
+        </is>
+      </c>
+      <c r="I100" s="3" t="inlineStr">
+        <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="J100" s="3" t="n"/>
+      <c r="K100" s="3" t="n"/>
+    </row>
+    <row r="101" hidden="1" ht="15.95" customHeight="1">
+      <c r="B101" s="2" t="inlineStr">
+        <is>
+          <t>LEC0739</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="inlineStr">
+        <is>
+          <t>739</t>
+        </is>
+      </c>
+      <c r="D101" s="3" t="inlineStr">
+        <is>
+          <t>lec739.ipynb</t>
+        </is>
+      </c>
+      <c r="E101" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\playground\scratch\lec739.ipynb</t>
+        </is>
+      </c>
+      <c r="F101" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G101" s="3" t="inlineStr">
+        <is>
+          <t>Stack</t>
+        </is>
+      </c>
+      <c r="H101" s="3" t="inlineStr">
+        <is>
+          <t>Monotonic Stack</t>
+        </is>
+      </c>
+      <c r="I101" s="3" t="inlineStr">
+        <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="J101" s="3" t="n"/>
+      <c r="K101" s="3" t="n"/>
+    </row>
+    <row r="102" hidden="1" ht="15.95" customHeight="1">
+      <c r="B102" s="2" t="inlineStr">
+        <is>
+          <t>LEC0901</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="inlineStr">
+        <is>
+          <t>901</t>
+        </is>
+      </c>
+      <c r="D102" s="3" t="inlineStr">
+        <is>
+          <t>LEC901.ipynb</t>
+        </is>
+      </c>
+      <c r="E102" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\playground\LEC\Monotonic_Stack\LEC901.ipynb</t>
+        </is>
+      </c>
+      <c r="F102" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G102" s="3" t="inlineStr">
+        <is>
+          <t>Stack</t>
+        </is>
+      </c>
+      <c r="H102" s="3" t="inlineStr">
+        <is>
+          <t>Monotonic Stack</t>
+        </is>
+      </c>
+      <c r="I102" s="3" t="inlineStr">
+        <is>
+          <t>Design</t>
+        </is>
+      </c>
+      <c r="J102" s="3" t="n"/>
+      <c r="K102" s="3" t="n"/>
+    </row>
+    <row r="103" hidden="1">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B103" s="9" t="inlineStr">
+        <is>
+          <t>LC0083</t>
+        </is>
+      </c>
+      <c r="C103" s="9" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Remove Duplicates from Sorted List</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\001Study\LEC.md</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>1</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Linked List</t>
+        </is>
+      </c>
+    </row>
+    <row r="104" hidden="1">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B104" s="9" t="inlineStr">
+        <is>
+          <t>LC0142</t>
+        </is>
+      </c>
+      <c r="C104" s="9" t="inlineStr">
+        <is>
+          <t>142</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Linked List Cycle II</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\001Study\LEC.md</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>2</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Linked List</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Two Pointers</t>
+        </is>
+      </c>
+    </row>
+    <row r="105" hidden="1">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B105" s="9" t="inlineStr">
+        <is>
+          <t>LC0143</t>
+        </is>
+      </c>
+      <c r="C105" s="9" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Reorder List</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\001Study\LEC.md</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>2</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Linked List</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Two Pointers</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Stack</t>
+        </is>
+      </c>
+    </row>
+    <row r="106" hidden="1">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B106" s="9" t="inlineStr">
+        <is>
+          <t>LC0203</t>
+        </is>
+      </c>
+      <c r="C106" s="9" t="inlineStr">
+        <is>
+          <t>203</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Remove Linked List Elements</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\001Study\LEC.md</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>1</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Linked List</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Recursion</t>
+        </is>
+      </c>
+    </row>
+    <row r="107" hidden="1">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B107" s="9" t="inlineStr">
+        <is>
+          <t>LC0876</t>
+        </is>
+      </c>
+      <c r="C107" s="9" t="inlineStr">
+        <is>
+          <t>876</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Middle of the Linked List</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\001Study\LEC.md</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>1</v>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Linked List</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Two Pointers</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K98">
+  <autoFilter ref="A1:K107">
+    <filterColumn colId="0" hiddenButton="0" showButton="1">
+      <filters blank="1"/>
+    </filterColumn>
     <filterColumn colId="5" hiddenButton="0" showButton="1">
       <filters>
-        <filter val="2"/>
+        <filter val="3"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Quick Update 2026-02-25 03:21
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -2776,6 +2776,11 @@
       <c r="K52" s="3" t="n"/>
     </row>
     <row r="53" ht="15.95" customHeight="1">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B53" s="2" t="inlineStr">
         <is>
           <t>LC0167</t>
@@ -2797,16 +2802,16 @@
         </is>
       </c>
       <c r="F53" s="6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G53" s="3" t="inlineStr">
         <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
           <t>Two Pointers</t>
-        </is>
-      </c>
-      <c r="H53" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
         </is>
       </c>
       <c r="I53" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Quick Update 2026-02-25 03:30
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -1037,7 +1037,7 @@
       </c>
       <c r="K11" s="3" t="n"/>
     </row>
-    <row r="12" ht="15.95" customHeight="1">
+    <row r="12" hidden="1" ht="15.95" customHeight="1">
       <c r="A12" t="inlineStr">
         <is>
           <t>x</t>
@@ -1084,7 +1084,7 @@
       <c r="J12" s="3" t="n"/>
       <c r="K12" s="3" t="n"/>
     </row>
-    <row r="13" ht="15.95" customHeight="1">
+    <row r="13" hidden="1" ht="15.95" customHeight="1">
       <c r="A13" t="inlineStr">
         <is>
           <t>x</t>
@@ -1439,7 +1439,12 @@
       <c r="J20" s="3" t="n"/>
       <c r="K20" s="3" t="n"/>
     </row>
-    <row r="21" hidden="1" ht="15.95" customHeight="1">
+    <row r="21" ht="15.95" customHeight="1">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
           <t>LC0053</t>
@@ -1461,21 +1466,21 @@
         </is>
       </c>
       <c r="F21" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G21" s="3" t="inlineStr">
         <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>Divide and Conquer</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
           <t>Dynamic Programming</t>
-        </is>
-      </c>
-      <c r="H21" s="3" t="inlineStr">
-        <is>
-          <t>Kadane's Algorithm</t>
-        </is>
-      </c>
-      <c r="I21" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
         </is>
       </c>
       <c r="J21" s="3" t="inlineStr">
@@ -2093,7 +2098,7 @@
       <c r="J35" s="3" t="n"/>
       <c r="K35" s="3" t="n"/>
     </row>
-    <row r="36" hidden="1" ht="15.95" customHeight="1">
+    <row r="36" ht="15.95" customHeight="1">
       <c r="B36" s="2" t="inlineStr">
         <is>
           <t>LC0102</t>
@@ -2135,7 +2140,7 @@
       <c r="J36" s="3" t="n"/>
       <c r="K36" s="3" t="n"/>
     </row>
-    <row r="37" hidden="1" ht="15.95" customHeight="1">
+    <row r="37" ht="15.95" customHeight="1">
       <c r="B37" s="2" t="inlineStr">
         <is>
           <t>LC0102</t>
@@ -2733,7 +2738,7 @@
       <c r="J51" s="3" t="n"/>
       <c r="K51" s="3" t="n"/>
     </row>
-    <row r="52" hidden="1" ht="15.95" customHeight="1">
+    <row r="52" ht="15.95" customHeight="1">
       <c r="B52" s="2" t="inlineStr">
         <is>
           <t>LC0155</t>
@@ -2775,7 +2780,7 @@
       <c r="J52" s="3" t="n"/>
       <c r="K52" s="3" t="n"/>
     </row>
-    <row r="53" ht="15.95" customHeight="1">
+    <row r="53" hidden="1" ht="15.95" customHeight="1">
       <c r="A53" t="inlineStr">
         <is>
           <t>x</t>
@@ -2822,7 +2827,7 @@
       <c r="J53" s="3" t="n"/>
       <c r="K53" s="3" t="n"/>
     </row>
-    <row r="54" hidden="1" ht="15.95" customHeight="1">
+    <row r="54" ht="15.95" customHeight="1">
       <c r="B54" s="2" t="inlineStr">
         <is>
           <t>LC0198</t>
@@ -3901,7 +3906,7 @@
       <c r="J78" s="3" t="n"/>
       <c r="K78" s="3" t="n"/>
     </row>
-    <row r="79" hidden="1" ht="15.95" customHeight="1">
+    <row r="79" ht="15.95" customHeight="1">
       <c r="B79" s="2" t="inlineStr">
         <is>
           <t>LC0674</t>
@@ -4072,7 +4077,7 @@
       <c r="J82" s="3" t="n"/>
       <c r="K82" s="3" t="n"/>
     </row>
-    <row r="83" hidden="1" ht="15.95" customHeight="1">
+    <row r="83" ht="15.95" customHeight="1">
       <c r="B83" s="2" t="inlineStr">
         <is>
           <t>LC0937</t>
@@ -4114,7 +4119,7 @@
       <c r="J83" s="3" t="n"/>
       <c r="K83" s="3" t="n"/>
     </row>
-    <row r="84" hidden="1" ht="15.95" customHeight="1">
+    <row r="84" ht="15.95" customHeight="1">
       <c r="B84" s="2" t="inlineStr">
         <is>
           <t>LC0937</t>
@@ -4286,7 +4291,7 @@
       </c>
       <c r="K87" s="3" t="n"/>
     </row>
-    <row r="88" hidden="1" ht="15.95" customHeight="1">
+    <row r="88" ht="15.95" customHeight="1">
       <c r="B88" s="2" t="inlineStr">
         <is>
           <t>LC2043</t>
@@ -4416,7 +4421,7 @@
       <c r="J90" s="3" t="n"/>
       <c r="K90" s="3" t="n"/>
     </row>
-    <row r="91" ht="15.95" customHeight="1">
+    <row r="91" hidden="1" ht="15.95" customHeight="1">
       <c r="A91" t="inlineStr">
         <is>
           <t>x</t>
@@ -4734,7 +4739,7 @@
       </c>
       <c r="K97" s="3" t="n"/>
     </row>
-    <row r="98" hidden="1" ht="15.95" customHeight="1">
+    <row r="98" ht="15.95" customHeight="1">
       <c r="B98" s="2" t="inlineStr">
         <is>
           <t>LEC0496</t>
@@ -5156,7 +5161,7 @@
     </filterColumn>
     <filterColumn colId="5" hiddenButton="0" showButton="1">
       <filters>
-        <filter val="3"/>
+        <filter val="4"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 10:03
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -2099,6 +2099,11 @@
       <c r="K35" s="3" t="n"/>
     </row>
     <row r="36" ht="15.95" customHeight="1">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
           <t>LC0102</t>
@@ -2120,7 +2125,7 @@
         </is>
       </c>
       <c r="F36" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G36" s="3" t="inlineStr">
         <is>
@@ -2129,18 +2134,23 @@
       </c>
       <c r="H36" s="3" t="inlineStr">
         <is>
-          <t>BFS</t>
+          <t>Breadth-First Search</t>
         </is>
       </c>
       <c r="I36" s="3" t="inlineStr">
         <is>
-          <t>Queue</t>
+          <t>Binary Tree</t>
         </is>
       </c>
       <c r="J36" s="3" t="n"/>
       <c r="K36" s="3" t="n"/>
     </row>
     <row r="37" ht="15.95" customHeight="1">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
           <t>LC0102</t>
@@ -2162,7 +2172,7 @@
         </is>
       </c>
       <c r="F37" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G37" s="3" t="inlineStr">
         <is>
@@ -2171,12 +2181,12 @@
       </c>
       <c r="H37" s="3" t="inlineStr">
         <is>
-          <t>BFS</t>
+          <t>Breadth-First Search</t>
         </is>
       </c>
       <c r="I37" s="3" t="inlineStr">
         <is>
-          <t>Queue</t>
+          <t>Binary Tree</t>
         </is>
       </c>
       <c r="J37" s="3" t="n"/>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 11:33
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -2749,6 +2749,11 @@
       <c r="K51" s="3" t="n"/>
     </row>
     <row r="52" ht="15.95" customHeight="1">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
           <t>LC0155</t>
@@ -2770,7 +2775,7 @@
         </is>
       </c>
       <c r="F52" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G52" s="3" t="inlineStr">
         <is>
@@ -2838,6 +2843,11 @@
       <c r="K53" s="3" t="n"/>
     </row>
     <row r="54" ht="15.95" customHeight="1">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
           <t>LC0198</t>
@@ -2859,16 +2869,16 @@
         </is>
       </c>
       <c r="F54" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G54" s="3" t="inlineStr">
         <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
           <t>Dynamic Programming</t>
-        </is>
-      </c>
-      <c r="H54" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
         </is>
       </c>
       <c r="I54" s="3" t="n"/>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 12:14
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -3927,6 +3927,11 @@
       <c r="K78" s="3" t="n"/>
     </row>
     <row r="79" ht="15.95" customHeight="1">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B79" s="2" t="inlineStr">
         <is>
           <t>LC0674</t>
@@ -3948,11 +3953,11 @@
         </is>
       </c>
       <c r="F79" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G79" s="3" t="inlineStr">
         <is>
-          <t>Dynamic Programming</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H79" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Quick Update 2026-02-25 12:49
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -4103,6 +4103,11 @@
       <c r="K82" s="3" t="n"/>
     </row>
     <row r="83" ht="15.95" customHeight="1">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B83" s="2" t="inlineStr">
         <is>
           <t>LC0937</t>
@@ -4124,27 +4129,32 @@
         </is>
       </c>
       <c r="F83" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G83" s="3" t="inlineStr">
         <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="H83" s="3" t="inlineStr">
+        <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H83" s="3" t="inlineStr">
+      <c r="I83" s="3" t="inlineStr">
         <is>
           <t>Sorting</t>
-        </is>
-      </c>
-      <c r="I83" s="3" t="inlineStr">
-        <is>
-          <t>Custom Sort</t>
         </is>
       </c>
       <c r="J83" s="3" t="n"/>
       <c r="K83" s="3" t="n"/>
     </row>
     <row r="84" ht="15.95" customHeight="1">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B84" s="2" t="inlineStr">
         <is>
           <t>LC0937</t>
@@ -4166,21 +4176,21 @@
         </is>
       </c>
       <c r="F84" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G84" s="3" t="inlineStr">
         <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="H84" s="3" t="inlineStr">
+        <is>
           <t>String</t>
         </is>
       </c>
-      <c r="H84" s="3" t="inlineStr">
+      <c r="I84" s="3" t="inlineStr">
         <is>
           <t>Sorting</t>
-        </is>
-      </c>
-      <c r="I84" s="3" t="inlineStr">
-        <is>
-          <t>Custom Sort</t>
         </is>
       </c>
       <c r="J84" s="3" t="n"/>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 12:52
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -4327,6 +4327,11 @@
       <c r="K87" s="3" t="n"/>
     </row>
     <row r="88" ht="15.95" customHeight="1">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B88" s="2" t="inlineStr">
         <is>
           <t>LC2043</t>
@@ -4348,7 +4353,7 @@
         </is>
       </c>
       <c r="F88" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G88" s="3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 19:08
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -4780,6 +4780,11 @@
       <c r="K97" s="3" t="n"/>
     </row>
     <row r="98" ht="15.95" customHeight="1">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B98" s="2" t="inlineStr">
         <is>
           <t>LEC0496</t>
@@ -4801,21 +4806,21 @@
         </is>
       </c>
       <c r="F98" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G98" s="3" t="inlineStr">
         <is>
-          <t>Stack</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H98" s="3" t="inlineStr">
         <is>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="I98" s="3" t="inlineStr">
+        <is>
           <t>Monotonic Stack</t>
-        </is>
-      </c>
-      <c r="I98" s="3" t="inlineStr">
-        <is>
-          <t>Hash Map</t>
         </is>
       </c>
       <c r="J98" s="3" t="n"/>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 19:48
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -1356,6 +1356,11 @@
       <c r="K18" s="3" t="n"/>
     </row>
     <row r="19" hidden="1" ht="15.95" customHeight="1">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
           <t>LC0049</t>
@@ -1377,27 +1382,32 @@
         </is>
       </c>
       <c r="F19" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G19" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
           <t>String</t>
-        </is>
-      </c>
-      <c r="I19" s="3" t="inlineStr">
-        <is>
-          <t>Sorting</t>
         </is>
       </c>
       <c r="J19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
     </row>
     <row r="20" hidden="1" ht="15.95" customHeight="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
           <t>LC0049</t>
@@ -1419,21 +1429,21 @@
         </is>
       </c>
       <c r="F20" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G20" s="3" t="inlineStr">
         <is>
-          <t>Hash Map</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H20" s="3" t="inlineStr">
         <is>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
           <t>String</t>
-        </is>
-      </c>
-      <c r="I20" s="3" t="inlineStr">
-        <is>
-          <t>Sorting</t>
         </is>
       </c>
       <c r="J20" s="3" t="n"/>
@@ -1805,6 +1815,11 @@
       <c r="K28" s="3" t="n"/>
     </row>
     <row r="29" hidden="1" ht="15.95" customHeight="1">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
           <t>LC0073</t>
@@ -1826,7 +1841,7 @@
         </is>
       </c>
       <c r="F29" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G29" s="3" t="inlineStr">
         <is>
@@ -1835,12 +1850,12 @@
       </c>
       <c r="H29" s="3" t="inlineStr">
         <is>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
           <t>Matrix</t>
-        </is>
-      </c>
-      <c r="I29" s="3" t="inlineStr">
-        <is>
-          <t>Hash Map</t>
         </is>
       </c>
       <c r="J29" s="3" t="n"/>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 20:26
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -1862,6 +1862,11 @@
       <c r="K29" s="3" t="n"/>
     </row>
     <row r="30" hidden="1" ht="15.95" customHeight="1">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
           <t>LC0074</t>
@@ -1883,27 +1888,32 @@
         </is>
       </c>
       <c r="F30" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G30" s="3" t="inlineStr">
         <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
           <t>Binary Search</t>
         </is>
       </c>
-      <c r="H30" s="3" t="inlineStr">
+      <c r="I30" s="3" t="inlineStr">
         <is>
           <t>Matrix</t>
-        </is>
-      </c>
-      <c r="I30" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
         </is>
       </c>
       <c r="J30" s="3" t="n"/>
       <c r="K30" s="3" t="n"/>
     </row>
     <row r="31" hidden="1" ht="15.95" customHeight="1">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
           <t>LC0074</t>
@@ -1925,27 +1935,32 @@
         </is>
       </c>
       <c r="F31" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G31" s="3" t="inlineStr">
         <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
           <t>Binary Search</t>
         </is>
       </c>
-      <c r="H31" s="3" t="inlineStr">
+      <c r="I31" s="3" t="inlineStr">
         <is>
           <t>Matrix</t>
-        </is>
-      </c>
-      <c r="I31" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
         </is>
       </c>
       <c r="J31" s="3" t="n"/>
       <c r="K31" s="3" t="n"/>
     </row>
     <row r="32" hidden="1" ht="15.95" customHeight="1">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
           <t>LC0074</t>
@@ -1967,21 +1982,21 @@
         </is>
       </c>
       <c r="F32" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G32" s="3" t="inlineStr">
         <is>
+          <t>Array</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
           <t>Binary Search</t>
         </is>
       </c>
-      <c r="H32" s="3" t="inlineStr">
+      <c r="I32" s="3" t="inlineStr">
         <is>
           <t>Matrix</t>
-        </is>
-      </c>
-      <c r="I32" s="3" t="inlineStr">
-        <is>
-          <t>Array</t>
         </is>
       </c>
       <c r="J32" s="3" t="n"/>

</xml_diff>

<commit_message>
Quick Update 2026-02-25 20:49
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -2399,6 +2399,11 @@
       <c r="K41" s="3" t="n"/>
     </row>
     <row r="42" hidden="1" ht="15.95" customHeight="1">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
           <t>LC0128</t>
@@ -2420,16 +2425,16 @@
         </is>
       </c>
       <c r="F42" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G42" s="3" t="inlineStr">
         <is>
-          <t>Hash Set</t>
+          <t>Array</t>
         </is>
       </c>
       <c r="H42" s="3" t="inlineStr">
         <is>
-          <t>Array</t>
+          <t>Hash Table</t>
         </is>
       </c>
       <c r="I42" s="3" t="inlineStr">

</xml_diff>

<commit_message>
Quick Update 2026-02-26 00:54
</commit_message>
<xml_diff>
--- a/practice/leetcode_files.xlsx
+++ b/practice/leetcode_files.xlsx
@@ -724,6 +724,11 @@
       <c r="K4" s="3" t="n"/>
     </row>
     <row r="5" hidden="1" ht="15.95" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
           <t>LC0003</t>
@@ -745,113 +750,123 @@
         </is>
       </c>
       <c r="F5" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5" s="3" t="inlineStr">
         <is>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
           <t>Sliding Window</t>
         </is>
       </c>
-      <c r="H5" s="3" t="inlineStr">
-        <is>
-          <t>Hash Map</t>
-        </is>
-      </c>
-      <c r="I5" s="3" t="inlineStr">
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>Two Pointers</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="n"/>
+    </row>
+    <row r="6" hidden="1" ht="15.95" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>LC0003</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>00019_LeetCode3_LongestSubstringWithoutRepeatingCharacters.ipynb</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00019_LeetCode3_LongestSubstringWithoutRepeatingCharacters.ipynb</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="J5" s="3" t="inlineStr">
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>Sliding Window</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
         <is>
           <t>Two Pointers</t>
         </is>
       </c>
-      <c r="K5" s="3" t="n"/>
-    </row>
-    <row r="6" hidden="1" ht="15.95" customHeight="1">
-      <c r="B6" s="2" t="inlineStr">
+      <c r="K6" s="3" t="n"/>
+    </row>
+    <row r="7" hidden="1" ht="15.95" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>LC0003</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>00019_LeetCode3_LongestSubstringWithoutRepeatingCharacters.ipynb</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>C:\pyproj\Study\CapitalOnePython\Leets_Jupyter\00019_LeetCode3_LongestSubstringWithoutRepeatingCharacters.ipynb</t>
-        </is>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G6" s="3" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>000039.LC0003.longest-substr-no-repeat.redo.py</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>C:\DataMajor\practice\000039.LC0003.longest-substr-no-repeat.redo.py</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>Hash Table</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
         <is>
           <t>Sliding Window</t>
-        </is>
-      </c>
-      <c r="H6" s="3" t="inlineStr">
-        <is>
-          <t>Hash Map</t>
-        </is>
-      </c>
-      <c r="I6" s="3" t="inlineStr">
-        <is>
-          <t>String</t>
-        </is>
-      </c>
-      <c r="J6" s="3" t="inlineStr">
-        <is>
-          <t>Two Pointers</t>
-        </is>
-      </c>
-      <c r="K6" s="3" t="n"/>
-    </row>
-    <row r="7" hidden="1" ht="15.95" customHeight="1">
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>LC0003</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>000039.LC0003.longest-substr-no-repeat.redo.py</t>
-        </is>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
-        <is>
-          <t>C:\DataMajor\practice\000039.LC0003.longest-substr-no-repeat.redo.py</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>Sliding Window</t>
-        </is>
-      </c>
-      <c r="H7" s="3" t="inlineStr">
-        <is>
-          <t>Hash Map</t>
-        </is>
-      </c>
-      <c r="I7" s="3" t="inlineStr">
-        <is>
-          <t>String</t>
         </is>
       </c>
       <c r="J7" s="3" t="inlineStr">

</xml_diff>